<commit_message>
Modified pbs and runner scripts for keldysh energy window.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>L</t>
   </si>
@@ -37,6 +38,36 @@
   </si>
   <si>
     <t xml:space="preserve">Size Complex (in GB)</t>
+  </si>
+  <si>
+    <t>Ham/Eigvecs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G Sym</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C_ab</t>
+  </si>
+  <si>
+    <t>C_gg</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G Asym</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -78,7 +109,9 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,19 +775,287 @@
         <f>B3*B4*B6/(2^30)</f>
         <v>5.9604644775390625</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f>C3*C4*C6/(2^30)</f>
         <v>0.171661376953125</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f>D3*D4*D6/(2^30)</f>
         <v>4.8883259296417236</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f>E3*E4*E6/(2^30)</f>
         <v>3.35693359375</v>
       </c>
     </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25"/>
+    <row r="18" ht="14.25"/>
+    <row r="19" ht="14.25"/>
+    <row r="20" ht="14.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <f>SUM(A21:G21)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <f>SUM(A22:G22)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <f>SUM(A23:G23)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <f>SUM(A24:G24)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25"/>
+    <row r="26" ht="14.25"/>
+    <row r="27" ht="14.25"/>
+    <row r="28" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Added program to average the batches for the keldysh G_R G_R*.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -3,18 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>L</t>
   </si>
@@ -38,6 +40,63 @@
   </si>
   <si>
     <t xml:space="preserve">Size Complex (in GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For 24 L^2 Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Size L^2xL^2 (in GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complex Size (in GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time / Dis (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time / Dis (hr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 Dis Time (days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batches Need (for 72 hr runtime)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size Needed Per Param Per Bin (in GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Energy Bins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Params</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Size Needed (in GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Size Needed (in TB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Size Needed (in GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Size Needed (in TB)</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time/ Dis (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIme / Dis (hr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 Dis Time (hr)</t>
   </si>
   <si>
     <t>Ham/Eigvecs</t>
@@ -105,13 +164,22 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,6 +712,9 @@
       <c r="E1" s="1">
         <v>80</v>
       </c>
+      <c r="F1">
+        <v>60</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
@@ -665,6 +736,10 @@
         <f>E1*E1</f>
         <v>6400</v>
       </c>
+      <c r="F2" s="2">
+        <f>F1*F1</f>
+        <v>3600</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
@@ -686,6 +761,10 @@
         <f>2*E2</f>
         <v>12800</v>
       </c>
+      <c r="F3" s="2">
+        <f>2*F2</f>
+        <v>7200</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
@@ -707,6 +786,10 @@
         <f>2*E2</f>
         <v>12800</v>
       </c>
+      <c r="F4" s="2">
+        <f>2*F2</f>
+        <v>7200</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
@@ -716,13 +799,16 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -735,57 +821,150 @@
       </c>
       <c r="C6">
         <f>2*C5</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <f>2*D5</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <f>2*E5</f>
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="F6" s="2">
+        <f>2*F5</f>
+        <v>16</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <f>B3*B4*B5/(2^30)</f>
         <v>2.9802322387695312</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <f>C3*C4*C5/(2^30)</f>
-        <v>0.0858306884765625</v>
-      </c>
-      <c r="D7" s="2">
+        <v>0.0762939453125</v>
+      </c>
+      <c r="D7" s="3">
         <f>D3*D4*D5/(2^30)</f>
-        <v>2.4441629648208618</v>
-      </c>
-      <c r="E7" s="2">
+        <v>1.9553303718566895</v>
+      </c>
+      <c r="E7" s="3">
         <f>E3*E4*E5/(2^30)</f>
-        <v>1.678466796875</v>
+        <v>1.220703125</v>
+      </c>
+      <c r="F7" s="3">
+        <f>F3*F4*F5/(2^30)</f>
+        <v>0.38623809814453125</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <f>B3*B4*B6/(2^30)</f>
         <v>5.9604644775390625</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <f>C3*C4*C6/(2^30)</f>
-        <v>0.171661376953125</v>
-      </c>
-      <c r="D8" s="2">
+        <v>0.152587890625</v>
+      </c>
+      <c r="D8" s="3">
         <f>D3*D4*D6/(2^30)</f>
-        <v>4.8883259296417236</v>
-      </c>
-      <c r="E8" s="2">
+        <v>3.9106607437133789</v>
+      </c>
+      <c r="E8" s="3">
         <f>E3*E4*E6/(2^30)</f>
-        <v>3.35693359375</v>
+        <v>2.44140625</v>
+      </c>
+      <c r="F8" s="3">
+        <f>F3*F4*F6/(2^30)</f>
+        <v>0.7724761962890625</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <f>6*B7</f>
+        <v>17.881393432617188</v>
+      </c>
+      <c r="C11">
+        <f>6*C7</f>
+        <v>0.457763671875</v>
+      </c>
+      <c r="D11">
+        <f>6*D7</f>
+        <v>11.731982231140137</v>
+      </c>
+      <c r="E11">
+        <f>6*E7</f>
+        <v>7.32421875</v>
+      </c>
+      <c r="F11" s="2">
+        <f>6*F7</f>
+        <v>2.3174285888671875</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14">
+        <f>50*(4+2)*B7*2</f>
+        <v>1788.1393432617188</v>
+      </c>
+      <c r="C14">
+        <f>50*(4+2)*C7*2</f>
+        <v>45.7763671875</v>
+      </c>
+      <c r="D14">
+        <f>50*(4+2)*D7*2</f>
+        <v>1173.1982231140137</v>
+      </c>
+      <c r="E14">
+        <f>50*(4+2)*E7*2</f>
+        <v>732.421875</v>
+      </c>
+      <c r="F14" s="2">
+        <f>50*(4+2)*F7*2</f>
+        <v>231.74285888671875</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15">
+        <f>B14*18/1024</f>
+        <v>31.4321368932724</v>
+      </c>
+      <c r="C15">
+        <f>C14*18/1024</f>
+        <v>0.80466270446777344</v>
+      </c>
+      <c r="D15">
+        <f>D14*18/1024</f>
+        <v>20.622625015676022</v>
+      </c>
+      <c r="E15">
+        <f>E14*18/1024</f>
+        <v>12.874603271484375</v>
+      </c>
+      <c r="F15" s="2">
+        <f>F14*18/1024</f>
+        <v>4.073604941368103</v>
       </c>
     </row>
   </sheetData>
@@ -800,6 +979,1195 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="10.57421875"/>
+    <col customWidth="1" min="12" max="12" width="13.7109375"/>
+    <col bestFit="1" min="13" max="14" width="9.4609375"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="1" ht="85.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6">
+        <f>A2^4*8/2^30</f>
+        <v>0.019073486328125</v>
+      </c>
+      <c r="C2" s="6">
+        <f>4*B2</f>
+        <v>0.0762939453125</v>
+      </c>
+      <c r="D2" s="6">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7">
+        <f>D2/60</f>
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="F2" s="6">
+        <f>D2*100/(60*24)</f>
+        <v>1.1805555555555556</v>
+      </c>
+      <c r="G2" s="6">
+        <f>CEILING(MAX(F2/3,1),1)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6">
+        <f>H2*G2*B2</f>
+        <v>0.11444091796875</v>
+      </c>
+      <c r="J2" s="6">
+        <v>50</v>
+      </c>
+      <c r="K2" s="6">
+        <v>18</v>
+      </c>
+      <c r="L2" s="6">
+        <f>I2*J2*K2</f>
+        <v>102.996826171875</v>
+      </c>
+      <c r="M2" s="6">
+        <f>L2/1024</f>
+        <v>0.10058283805847168</v>
+      </c>
+      <c r="N2" s="6">
+        <f>L2/G2</f>
+        <v>102.996826171875</v>
+      </c>
+      <c r="O2" s="6">
+        <f>N2/1024</f>
+        <v>0.10058283805847168</v>
+      </c>
+      <c r="P2">
+        <f>G2*K2</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3" s="6">
+        <f>A3^4*8/2^30</f>
+        <v>0.046566128730773926</v>
+      </c>
+      <c r="C3" s="6">
+        <f>4*B3</f>
+        <v>0.1862645149230957</v>
+      </c>
+      <c r="D3" s="6">
+        <f>$D$2*(A3/$A$2)^6</f>
+        <v>64.849853515625</v>
+      </c>
+      <c r="E3" s="7">
+        <f>D3/60</f>
+        <v>1.0808308919270833</v>
+      </c>
+      <c r="F3" s="6">
+        <f>D3*100/(60*24)</f>
+        <v>4.5034620496961804</v>
+      </c>
+      <c r="G3" s="6">
+        <f>CEILING(MAX(F3/3,1),1)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>6</v>
+      </c>
+      <c r="I3" s="6">
+        <f>H3*G3*B3</f>
+        <v>0.55879354476928711</v>
+      </c>
+      <c r="J3" s="6">
+        <v>50</v>
+      </c>
+      <c r="K3" s="6">
+        <v>18</v>
+      </c>
+      <c r="L3" s="6">
+        <f>I3*J3*K3</f>
+        <v>502.9141902923584</v>
+      </c>
+      <c r="M3" s="6">
+        <f>L3/1024</f>
+        <v>0.49112713895738125</v>
+      </c>
+      <c r="N3" s="6">
+        <f>L3/G3</f>
+        <v>251.4570951461792</v>
+      </c>
+      <c r="O3" s="6">
+        <f>N3/1024</f>
+        <v>0.24556356947869062</v>
+      </c>
+      <c r="P3">
+        <f>G3*K3</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4">
+        <v>60</v>
+      </c>
+      <c r="B4" s="6">
+        <f>A4^4*8/2^30</f>
+        <v>0.096559524536132812</v>
+      </c>
+      <c r="C4" s="6">
+        <f>4*B4</f>
+        <v>0.38623809814453125</v>
+      </c>
+      <c r="D4" s="6">
+        <f>$D$2*(A4/$A$2)^6</f>
+        <v>193.640625</v>
+      </c>
+      <c r="E4" s="7">
+        <f>D4/60</f>
+        <v>3.2273437500000002</v>
+      </c>
+      <c r="F4" s="6">
+        <f>D4*100/(60*24)</f>
+        <v>13.447265625</v>
+      </c>
+      <c r="G4" s="6">
+        <f>CEILING(MAX(F4/3,1),1)</f>
+        <v>5</v>
+      </c>
+      <c r="H4" s="6">
+        <v>6</v>
+      </c>
+      <c r="I4" s="6">
+        <f>H4*G4*B4</f>
+        <v>2.8967857360839844</v>
+      </c>
+      <c r="J4" s="6">
+        <v>50</v>
+      </c>
+      <c r="K4" s="6">
+        <v>18</v>
+      </c>
+      <c r="L4" s="6">
+        <f>I4*J4*K4</f>
+        <v>2607.1071624755859</v>
+      </c>
+      <c r="M4" s="6">
+        <f>L4/1024</f>
+        <v>2.5460030883550644</v>
+      </c>
+      <c r="N4" s="6">
+        <f>L4/G4</f>
+        <v>521.42143249511719</v>
+      </c>
+      <c r="O4" s="6">
+        <f>N4/1024</f>
+        <v>0.50920061767101288</v>
+      </c>
+      <c r="P4">
+        <f>G4*K4</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5">
+        <v>70</v>
+      </c>
+      <c r="B5" s="6">
+        <f>A5^4*8/2^30</f>
+        <v>0.17888844013214111</v>
+      </c>
+      <c r="C5" s="6">
+        <f>4*B5</f>
+        <v>0.71555376052856445</v>
+      </c>
+      <c r="D5" s="6">
+        <f>$D$2*(A5/$A$2)^6</f>
+        <v>488.289306640625</v>
+      </c>
+      <c r="E5" s="7">
+        <f>D5/60</f>
+        <v>8.1381551106770829</v>
+      </c>
+      <c r="F5" s="6">
+        <f>D5*100/(60*24)</f>
+        <v>33.908979627821182</v>
+      </c>
+      <c r="G5" s="6">
+        <f>CEILING(MAX(F5/3,1),1)</f>
+        <v>12</v>
+      </c>
+      <c r="H5" s="6">
+        <v>6</v>
+      </c>
+      <c r="I5" s="6">
+        <f>H5*G5*B5</f>
+        <v>12.87996768951416</v>
+      </c>
+      <c r="J5" s="6">
+        <v>50</v>
+      </c>
+      <c r="K5" s="6">
+        <v>18</v>
+      </c>
+      <c r="L5" s="6">
+        <f>I5*J5*K5</f>
+        <v>11591.970920562744</v>
+      </c>
+      <c r="M5" s="6">
+        <f>L5/1024</f>
+        <v>11.320284102112055</v>
+      </c>
+      <c r="N5" s="6">
+        <f>L5/G5</f>
+        <v>965.99757671356201</v>
+      </c>
+      <c r="O5" s="6">
+        <f>N5/1024</f>
+        <v>0.9433570085093379</v>
+      </c>
+      <c r="P5">
+        <f>G5*K5</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6">
+        <v>80</v>
+      </c>
+      <c r="B6" s="6">
+        <f>A6^4*8/2^30</f>
+        <v>0.30517578125</v>
+      </c>
+      <c r="C6" s="6">
+        <f>4*B6</f>
+        <v>1.220703125</v>
+      </c>
+      <c r="D6" s="6">
+        <f>$D$2*(A6/$A$2)^6</f>
+        <v>1088</v>
+      </c>
+      <c r="E6" s="7">
+        <f>D6/60</f>
+        <v>18.133333333333333</v>
+      </c>
+      <c r="F6" s="6">
+        <f>D6*100/(60*24)</f>
+        <v>75.555555555555557</v>
+      </c>
+      <c r="G6" s="6">
+        <f>CEILING(MAX(F6/3,1),1)</f>
+        <v>26</v>
+      </c>
+      <c r="H6" s="6">
+        <v>6</v>
+      </c>
+      <c r="I6" s="6">
+        <f>H6*G6*B6</f>
+        <v>47.607421875</v>
+      </c>
+      <c r="J6" s="6">
+        <v>50</v>
+      </c>
+      <c r="K6" s="6">
+        <v>18</v>
+      </c>
+      <c r="L6" s="6">
+        <f>I6*J6*K6</f>
+        <v>42846.6796875</v>
+      </c>
+      <c r="M6" s="6">
+        <f>L6/1024</f>
+        <v>41.842460632324219</v>
+      </c>
+      <c r="N6" s="6">
+        <f>L6/G6</f>
+        <v>1647.94921875</v>
+      </c>
+      <c r="O6" s="6">
+        <f>N6/1024</f>
+        <v>1.6093254089355469</v>
+      </c>
+      <c r="P6">
+        <f>G6*K6</f>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7">
+        <v>90</v>
+      </c>
+      <c r="B7" s="6">
+        <f>A7^4*8/2^30</f>
+        <v>0.48883259296417236</v>
+      </c>
+      <c r="C7" s="6">
+        <f>4*B7</f>
+        <v>1.9553303718566895</v>
+      </c>
+      <c r="D7" s="6">
+        <f>$D$2*(A7/$A$2)^6</f>
+        <v>2205.687744140625</v>
+      </c>
+      <c r="E7" s="7">
+        <f>D7/60</f>
+        <v>36.761462402343753</v>
+      </c>
+      <c r="F7" s="6">
+        <f>D7*100/(60*24)</f>
+        <v>153.17276000976562</v>
+      </c>
+      <c r="G7" s="6">
+        <f>CEILING(MAX(F7/3,1),1)</f>
+        <v>52</v>
+      </c>
+      <c r="H7" s="6">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6">
+        <f>H7*G7*B7</f>
+        <v>152.51576900482178</v>
+      </c>
+      <c r="J7" s="6">
+        <v>50</v>
+      </c>
+      <c r="K7" s="6">
+        <v>18</v>
+      </c>
+      <c r="L7" s="6">
+        <f>I7*J7*K7</f>
+        <v>137264.1921043396</v>
+      </c>
+      <c r="M7" s="6">
+        <f>L7/1024</f>
+        <v>134.04706260189414</v>
+      </c>
+      <c r="N7" s="6">
+        <f>L7/G7</f>
+        <v>2639.6960020065308</v>
+      </c>
+      <c r="O7" s="6">
+        <f>N7/1024</f>
+        <v>2.5778281269595027</v>
+      </c>
+      <c r="P7">
+        <f>G7*K7</f>
+        <v>936</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8" s="6">
+        <f>A8^4*8/2^30</f>
+        <v>0.74505805969238281</v>
+      </c>
+      <c r="C8" s="6">
+        <f>4*B8</f>
+        <v>2.9802322387695312</v>
+      </c>
+      <c r="D8" s="6">
+        <f>$D$2*(A8/$A$2)^6</f>
+        <v>4150.390625</v>
+      </c>
+      <c r="E8" s="7">
+        <f>D8/60</f>
+        <v>69.173177083333329</v>
+      </c>
+      <c r="F8" s="6">
+        <f>D8*100/(60*24)</f>
+        <v>288.22157118055554</v>
+      </c>
+      <c r="G8" s="6">
+        <f>CEILING(MAX(F8/3,1),1)</f>
+        <v>97</v>
+      </c>
+      <c r="H8" s="6">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6">
+        <f>H8*G8*B8</f>
+        <v>433.6237907409668</v>
+      </c>
+      <c r="J8" s="6">
+        <v>50</v>
+      </c>
+      <c r="K8" s="6">
+        <v>18</v>
+      </c>
+      <c r="L8" s="6">
+        <f>I8*J8*K8</f>
+        <v>390261.41166687012</v>
+      </c>
+      <c r="M8" s="6">
+        <f>L8/1024</f>
+        <v>381.11465983092785</v>
+      </c>
+      <c r="N8" s="6">
+        <f>L8/G8</f>
+        <v>4023.3135223388672</v>
+      </c>
+      <c r="O8" s="6">
+        <f>N8/1024</f>
+        <v>3.92901711165905</v>
+      </c>
+      <c r="P8">
+        <f>G8*K8</f>
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9">
+        <v>110</v>
+      </c>
+      <c r="B9" s="6">
+        <f>A9^4*8/2^30</f>
+        <v>1.0908395051956177</v>
+      </c>
+      <c r="C9" s="6">
+        <f>4*B9</f>
+        <v>4.3633580207824707</v>
+      </c>
+      <c r="D9" s="6">
+        <f>$D$2*(A9/$A$2)^6</f>
+        <v>7352.670166015625</v>
+      </c>
+      <c r="E9" s="7">
+        <f>D9/60</f>
+        <v>122.54450276692708</v>
+      </c>
+      <c r="F9" s="6">
+        <f>D9*100/(60*24)</f>
+        <v>510.60209486219617</v>
+      </c>
+      <c r="G9" s="6">
+        <f>CEILING(MAX(F9/3,1),1)</f>
+        <v>171</v>
+      </c>
+      <c r="H9" s="6">
+        <v>6</v>
+      </c>
+      <c r="I9" s="6">
+        <f>H9*G9*B9</f>
+        <v>1119.2013323307037</v>
+      </c>
+      <c r="J9" s="6">
+        <v>50</v>
+      </c>
+      <c r="K9" s="6">
+        <v>18</v>
+      </c>
+      <c r="L9" s="6">
+        <f>I9*J9*K9</f>
+        <v>1007281.1990976334</v>
+      </c>
+      <c r="M9" s="6">
+        <f>L9/1024</f>
+        <v>983.67304599378258</v>
+      </c>
+      <c r="N9" s="6">
+        <f>L9/G9</f>
+        <v>5890.5333280563354</v>
+      </c>
+      <c r="O9" s="6">
+        <f>N9/1024</f>
+        <v>5.7524739531800151</v>
+      </c>
+      <c r="P9">
+        <f>G9*K9</f>
+        <v>3078</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10">
+        <v>120</v>
+      </c>
+      <c r="B10" s="6">
+        <f>A10^4*8/2^30</f>
+        <v>1.544952392578125</v>
+      </c>
+      <c r="C10" s="6">
+        <f>4*B10</f>
+        <v>6.1798095703125</v>
+      </c>
+      <c r="D10" s="6">
+        <f>$D$2*(A10/$A$2)^6</f>
+        <v>12393</v>
+      </c>
+      <c r="E10" s="7">
+        <f>D10/60</f>
+        <v>206.55000000000001</v>
+      </c>
+      <c r="F10" s="6">
+        <f>D10*100/(60*24)</f>
+        <v>860.625</v>
+      </c>
+      <c r="G10" s="6">
+        <f>CEILING(MAX(F10/3,1),1)</f>
+        <v>287</v>
+      </c>
+      <c r="H10" s="6">
+        <v>6</v>
+      </c>
+      <c r="I10" s="6">
+        <f>H10*G10*B10</f>
+        <v>2660.4080200195312</v>
+      </c>
+      <c r="J10" s="6">
+        <v>50</v>
+      </c>
+      <c r="K10" s="6">
+        <v>18</v>
+      </c>
+      <c r="L10" s="6">
+        <f>I10*J10*K10</f>
+        <v>2394367.2180175781</v>
+      </c>
+      <c r="M10" s="6">
+        <f>L10/1024</f>
+        <v>2338.2492363452911</v>
+      </c>
+      <c r="N10" s="6">
+        <f>L10/G10</f>
+        <v>8342.742919921875</v>
+      </c>
+      <c r="O10" s="6">
+        <f>N10/1024</f>
+        <v>8.1472098827362061</v>
+      </c>
+      <c r="P10">
+        <f>G10*K10</f>
+        <v>5166</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11">
+        <v>130</v>
+      </c>
+      <c r="B11" s="6">
+        <f>A11^4*8/2^30</f>
+        <v>2.1279603242874146</v>
+      </c>
+      <c r="C11" s="6">
+        <f>4*B11</f>
+        <v>8.5118412971496582</v>
+      </c>
+      <c r="D11" s="6">
+        <f>$D$2*(A11/$A$2)^6</f>
+        <v>20033.142822265625</v>
+      </c>
+      <c r="E11" s="7">
+        <f>D11/60</f>
+        <v>333.88571370442708</v>
+      </c>
+      <c r="F11" s="6">
+        <f>D11*100/(60*24)</f>
+        <v>1391.1904737684463</v>
+      </c>
+      <c r="G11" s="6">
+        <f>CEILING(MAX(F11/3,1),1)</f>
+        <v>464</v>
+      </c>
+      <c r="H11" s="6">
+        <v>6</v>
+      </c>
+      <c r="I11" s="6">
+        <f>H11*G11*B11</f>
+        <v>5924.2415428161621</v>
+      </c>
+      <c r="J11" s="6">
+        <v>50</v>
+      </c>
+      <c r="K11" s="6">
+        <v>18</v>
+      </c>
+      <c r="L11" s="6">
+        <f>I11*J11*K11</f>
+        <v>5331817.3885345459</v>
+      </c>
+      <c r="M11" s="6">
+        <f>L11/1024</f>
+        <v>5206.8529184907675</v>
+      </c>
+      <c r="N11" s="6">
+        <f>L11/G11</f>
+        <v>11490.985751152039</v>
+      </c>
+      <c r="O11" s="6">
+        <f>N11/1024</f>
+        <v>11.221665772609413</v>
+      </c>
+      <c r="P11">
+        <f>G11*K11</f>
+        <v>8352</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12">
+        <v>140</v>
+      </c>
+      <c r="B12" s="6">
+        <f>A12^4*8/2^30</f>
+        <v>2.8622150421142578</v>
+      </c>
+      <c r="C12" s="6">
+        <f>4*B12</f>
+        <v>11.448860168457031</v>
+      </c>
+      <c r="D12" s="6">
+        <f>$D$2*(A12/$A$2)^6</f>
+        <v>31250.515625</v>
+      </c>
+      <c r="E12" s="7">
+        <f>D12/60</f>
+        <v>520.8419270833333</v>
+      </c>
+      <c r="F12" s="6">
+        <f>D12*100/(60*24)</f>
+        <v>2170.1746961805557</v>
+      </c>
+      <c r="G12" s="6">
+        <f>CEILING(MAX(F12/3,1),1)</f>
+        <v>724</v>
+      </c>
+      <c r="H12" s="6">
+        <v>6</v>
+      </c>
+      <c r="I12" s="6">
+        <f>H12*G12*B12</f>
+        <v>12433.462142944336</v>
+      </c>
+      <c r="J12" s="6">
+        <v>50</v>
+      </c>
+      <c r="K12" s="6">
+        <v>18</v>
+      </c>
+      <c r="L12" s="6">
+        <f>I12*J12*K12</f>
+        <v>11190115.928649902</v>
+      </c>
+      <c r="M12" s="6">
+        <f>L12/1024</f>
+        <v>10927.84758657217</v>
+      </c>
+      <c r="N12" s="6">
+        <f>L12/G12</f>
+        <v>15455.961227416992</v>
+      </c>
+      <c r="O12" s="6">
+        <f>N12/1024</f>
+        <v>15.093712136149406</v>
+      </c>
+      <c r="P12">
+        <f>G12*K12</f>
+        <v>13032</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13">
+        <v>150</v>
+      </c>
+      <c r="B13" s="6">
+        <f>A13^4*8/2^30</f>
+        <v>3.771856427192688</v>
+      </c>
+      <c r="C13" s="6">
+        <f>4*B13</f>
+        <v>15.087425708770752</v>
+      </c>
+      <c r="D13" s="6">
+        <f>$D$2*(A13/$A$2)^6</f>
+        <v>47275.543212890625</v>
+      </c>
+      <c r="E13" s="7">
+        <f>D13/60</f>
+        <v>787.92572021484375</v>
+      </c>
+      <c r="F13" s="6">
+        <f>D13*100/(60*24)</f>
+        <v>3283.0238342285156</v>
+      </c>
+      <c r="G13" s="6">
+        <f>CEILING(MAX(F13/3,1),1)</f>
+        <v>1095</v>
+      </c>
+      <c r="H13" s="6">
+        <v>6</v>
+      </c>
+      <c r="I13" s="6">
+        <f>H13*G13*B13</f>
+        <v>24781.09672665596</v>
+      </c>
+      <c r="J13" s="6">
+        <v>50</v>
+      </c>
+      <c r="K13" s="6">
+        <v>18</v>
+      </c>
+      <c r="L13" s="6">
+        <f>I13*J13*K13</f>
+        <v>22302987.053990364</v>
+      </c>
+      <c r="M13" s="6">
+        <f>L13/1024</f>
+        <v>21780.260794912465</v>
+      </c>
+      <c r="N13" s="6">
+        <f>L13/G13</f>
+        <v>20368.024706840515</v>
+      </c>
+      <c r="O13" s="6">
+        <f>N13/1024</f>
+        <v>19.890649127773941</v>
+      </c>
+      <c r="P13">
+        <f>G13*K13</f>
+        <v>19710</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14">
+        <v>76</v>
+      </c>
+      <c r="B14" s="6">
+        <f>A14^4*8/2^30</f>
+        <v>0.24856758117675781</v>
+      </c>
+      <c r="C14" s="6">
+        <f>4*B14</f>
+        <v>0.99427032470703125</v>
+      </c>
+      <c r="D14" s="6">
+        <f>$D$2*(A14/$A$2)^6</f>
+        <v>799.7799769999998</v>
+      </c>
+      <c r="E14" s="6">
+        <f>D14/60</f>
+        <v>13.32966628333333</v>
+      </c>
+      <c r="F14" s="6">
+        <f>D14*100/(60*24)</f>
+        <v>55.540276180555537</v>
+      </c>
+      <c r="G14" s="6">
+        <f>CEILING(MAX(F14/3,1),1)</f>
+        <v>19</v>
+      </c>
+      <c r="H14" s="6">
+        <v>6</v>
+      </c>
+      <c r="I14" s="6">
+        <f>H14*G14*B14</f>
+        <v>28.336704254150391</v>
+      </c>
+      <c r="J14" s="6">
+        <v>50</v>
+      </c>
+      <c r="K14" s="6">
+        <v>18</v>
+      </c>
+      <c r="L14" s="6">
+        <f>I14*J14*K14</f>
+        <v>25503.033828735352</v>
+      </c>
+      <c r="M14" s="6">
+        <f>L14/1024</f>
+        <v>24.905306473374367</v>
+      </c>
+      <c r="N14" s="6">
+        <f>L14/G14</f>
+        <v>1342.2649383544922</v>
+      </c>
+      <c r="O14" s="6">
+        <f>N14/1024</f>
+        <v>1.3108056038618088</v>
+      </c>
+      <c r="P14" s="2">
+        <f>G14*K14</f>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="2">
+        <v>60</v>
+      </c>
+      <c r="B15" s="6">
+        <f>A15^4*8/2^30</f>
+        <v>0.096559524536132812</v>
+      </c>
+      <c r="C15" s="6">
+        <f>4*B15</f>
+        <v>0.38623809814453125</v>
+      </c>
+      <c r="D15" s="6">
+        <f>$D$2*(A15/$A$2)^6</f>
+        <v>193.640625</v>
+      </c>
+      <c r="E15" s="6">
+        <f>D15/60</f>
+        <v>3.2273437500000002</v>
+      </c>
+      <c r="F15" s="6">
+        <f>D15*100/(60*24)</f>
+        <v>13.447265625</v>
+      </c>
+      <c r="G15" s="6">
+        <f>CEILING(MAX(F15/3,1),1)</f>
+        <v>5</v>
+      </c>
+      <c r="H15" s="6">
+        <v>6</v>
+      </c>
+      <c r="I15" s="6">
+        <f>H15*G15*B15</f>
+        <v>2.8967857360839844</v>
+      </c>
+      <c r="J15" s="6">
+        <v>50</v>
+      </c>
+      <c r="K15" s="6">
+        <v>18</v>
+      </c>
+      <c r="L15" s="6">
+        <f>I15*J15*K15</f>
+        <v>2607.1071624755859</v>
+      </c>
+      <c r="M15" s="6">
+        <f>L15/1024</f>
+        <v>2.5460030883550644</v>
+      </c>
+      <c r="N15" s="6">
+        <f>L15/G15</f>
+        <v>521.42143249511719</v>
+      </c>
+      <c r="O15" s="6">
+        <f>N15/1024</f>
+        <v>0.50920061767101288</v>
+      </c>
+      <c r="P15" s="2">
+        <f>G15*K15</f>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="15.140625"/>
+    <col customWidth="1" min="3" max="3" width="12.8515625"/>
+    <col bestFit="1" min="4" max="4" width="9.4609375"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2/60</f>
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="D2" s="3">
+        <f>C2*100</f>
+        <v>28.333333333333332</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2/24</f>
+        <v>1.1805555555555556</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="3">
+        <f>B2*(A3/A2)^6</f>
+        <v>4150.390625</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B3/60</f>
+        <v>69.173177083333329</v>
+      </c>
+      <c r="D3" s="3">
+        <f>C3*100</f>
+        <v>6917.317708333333</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3/24</f>
+        <v>288.22157118055554</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>50</v>
+      </c>
+      <c r="B4" s="3">
+        <f>B3*(A4/A3)^6</f>
+        <v>64.849853515625</v>
+      </c>
+      <c r="C4" s="3">
+        <f>B4/60</f>
+        <v>1.0808308919270833</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4*100</f>
+        <v>108.08308919270833</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4/24</f>
+        <v>4.5034620496961804</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5" s="3">
+        <f>B4*(A5/A4)^6</f>
+        <v>193.64062499999994</v>
+      </c>
+      <c r="C5" s="3">
+        <f>B5/60</f>
+        <v>3.2273437499999988</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5*100</f>
+        <v>322.73437499999989</v>
+      </c>
+      <c r="E5" s="3">
+        <f>D5/24</f>
+        <v>13.447265624999995</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3">
+        <f>B5*(A6/A5)^6</f>
+        <v>488.28930664062506</v>
+      </c>
+      <c r="C6" s="3">
+        <f>B6/60</f>
+        <v>8.1381551106770846</v>
+      </c>
+      <c r="D6" s="3">
+        <f>C6*100</f>
+        <v>813.81551106770848</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6/24</f>
+        <v>33.908979627821189</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3">
+        <f>B6*(A7/A6)^6</f>
+        <v>1087.9999999999998</v>
+      </c>
+      <c r="C7" s="3">
+        <f>B7/60</f>
+        <v>18.133333333333329</v>
+      </c>
+      <c r="D7" s="3">
+        <f>C7*100</f>
+        <v>1813.333333333333</v>
+      </c>
+      <c r="E7" s="3">
+        <f>D7/24</f>
+        <v>75.555555555555543</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>90</v>
+      </c>
+      <c r="B8" s="3">
+        <f>B7*(A8/A7)^6</f>
+        <v>2205.6877441406245</v>
+      </c>
+      <c r="C8" s="3">
+        <f>B8/60</f>
+        <v>36.761462402343746</v>
+      </c>
+      <c r="D8" s="3">
+        <f>C8*100</f>
+        <v>3676.1462402343745</v>
+      </c>
+      <c r="E8" s="3">
+        <f>D8/24</f>
+        <v>153.1727600097656</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B8*(A9/A8)^6</f>
+        <v>4150.390625</v>
+      </c>
+      <c r="C9" s="3">
+        <f>B9/60</f>
+        <v>69.173177083333329</v>
+      </c>
+      <c r="D9" s="3">
+        <f>C9*100</f>
+        <v>6917.317708333333</v>
+      </c>
+      <c r="E9" s="3">
+        <f>D9/24</f>
+        <v>288.22157118055554</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B9*(A10/A9)^6</f>
+        <v>7352.6701660156286</v>
+      </c>
+      <c r="C10" s="3">
+        <f>B10/60</f>
+        <v>122.54450276692714</v>
+      </c>
+      <c r="D10" s="3">
+        <f>C10*100</f>
+        <v>12254.450276692714</v>
+      </c>
+      <c r="E10" s="3">
+        <f>D10/24</f>
+        <v>510.60209486219645</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>120</v>
+      </c>
+      <c r="B11" s="3">
+        <f>B10*(A11/A10)^6</f>
+        <v>12393</v>
+      </c>
+      <c r="C11" s="3">
+        <f>B11/60</f>
+        <v>206.55000000000001</v>
+      </c>
+      <c r="D11" s="3">
+        <f>C11*100</f>
+        <v>20655</v>
+      </c>
+      <c r="E11" s="3">
+        <f>D11/24</f>
+        <v>860.625</v>
+      </c>
+    </row>
+    <row r="15"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -807,7 +2175,7 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -818,7 +2186,7 @@
     </row>
     <row r="2" ht="14.25">
       <c r="D2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -829,7 +2197,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="G3" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -840,7 +2208,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="G4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -851,7 +2219,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="G6" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -862,7 +2230,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="G7" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -873,7 +2241,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="G8" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -884,7 +2252,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="D10" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -895,7 +2263,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="G11" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -906,7 +2274,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="G12" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -917,34 +2285,34 @@
     </row>
     <row r="14" ht="14.25">
       <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="3">
+        <v>31</v>
+      </c>
+      <c r="H14" s="2">
         <v>1</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="3">
+        <v>32</v>
+      </c>
+      <c r="H15" s="2">
         <v>1</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="3">
+        <v>33</v>
+      </c>
+      <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>2</v>
       </c>
     </row>
@@ -953,25 +2321,25 @@
     <row r="19" ht="14.25"/>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" ht="14.25">

</xml_diff>

<commit_message>
Modified to generate and run PBS files.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -164,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -174,12 +175,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,7 +999,7 @@
       <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -1018,25 +1014,25 @@
       <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1044,60 +1040,60 @@
       <c r="A2">
         <v>40</v>
       </c>
-      <c r="B2" s="6">
-        <f>A2^4*8/2^30</f>
+      <c r="B2" s="5">
+        <f t="shared" ref="B2:B9" si="0">A2^4*8/2^30</f>
         <v>0.019073486328125</v>
       </c>
-      <c r="C2" s="6">
-        <f>4*B2</f>
+      <c r="C2" s="5">
+        <f t="shared" ref="C2:C9" si="1">4*B2</f>
         <v>0.0762939453125</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>17</v>
       </c>
-      <c r="E2" s="7">
-        <f>D2/60</f>
+      <c r="E2" s="5">
+        <f t="shared" ref="E2:E9" si="2">D2/60</f>
         <v>0.28333333333333333</v>
       </c>
-      <c r="F2" s="6">
-        <f>D2*100/(60*24)</f>
+      <c r="F2" s="5">
+        <f t="shared" ref="F2:F9" si="3">D2*100/(60*24)</f>
         <v>1.1805555555555556</v>
       </c>
-      <c r="G2" s="6">
-        <f>CEILING(MAX(F2/3,1),1)</f>
+      <c r="G2" s="5">
+        <f t="shared" ref="G2:G9" si="4">CEILING(MAX(F2/3,1),1)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>6</v>
       </c>
-      <c r="I2" s="6">
-        <f>H2*G2*B2</f>
+      <c r="I2" s="5">
+        <f t="shared" ref="I2:I9" si="5">H2*G2*B2</f>
         <v>0.11444091796875</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>50</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>18</v>
       </c>
-      <c r="L2" s="6">
-        <f>I2*J2*K2</f>
+      <c r="L2" s="5">
+        <f t="shared" ref="L2:L9" si="6">I2*J2*K2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="M2" s="6">
-        <f>L2/1024</f>
+      <c r="M2" s="5">
+        <f t="shared" ref="M2:M9" si="7">L2/1024</f>
         <v>0.10058283805847168</v>
       </c>
-      <c r="N2" s="6">
-        <f>L2/G2</f>
+      <c r="N2" s="5">
+        <f t="shared" ref="N2:N9" si="8">L2/G2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="O2" s="6">
-        <f>N2/1024</f>
+      <c r="O2" s="5">
+        <f t="shared" ref="O2:O9" si="9">N2/1024</f>
         <v>0.10058283805847168</v>
       </c>
       <c r="P2">
-        <f>G2*K2</f>
+        <f t="shared" ref="P2:P9" si="10">G2*K2</f>
         <v>18</v>
       </c>
     </row>
@@ -1105,61 +1101,61 @@
       <c r="A3">
         <v>50</v>
       </c>
-      <c r="B3" s="6">
-        <f>A3^4*8/2^30</f>
+      <c r="B3" s="5">
+        <f t="shared" si="0"/>
         <v>0.046566128730773926</v>
       </c>
-      <c r="C3" s="6">
-        <f>4*B3</f>
+      <c r="C3" s="5">
+        <f t="shared" si="1"/>
         <v>0.1862645149230957</v>
       </c>
-      <c r="D3" s="6">
-        <f>$D$2*(A3/$A$2)^6</f>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D9" si="11">$D$2*(A3/$A$2)^6</f>
         <v>64.849853515625</v>
       </c>
-      <c r="E3" s="7">
-        <f>D3/60</f>
+      <c r="E3" s="5">
+        <f t="shared" si="2"/>
         <v>1.0808308919270833</v>
       </c>
-      <c r="F3" s="6">
-        <f>D3*100/(60*24)</f>
+      <c r="F3" s="5">
+        <f t="shared" si="3"/>
         <v>4.5034620496961804</v>
       </c>
-      <c r="G3" s="6">
-        <f>CEILING(MAX(F3/3,1),1)</f>
+      <c r="G3" s="5">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>6</v>
       </c>
-      <c r="I3" s="6">
-        <f>H3*G3*B3</f>
+      <c r="I3" s="5">
+        <f t="shared" si="5"/>
         <v>0.55879354476928711</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>50</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>18</v>
       </c>
-      <c r="L3" s="6">
-        <f>I3*J3*K3</f>
+      <c r="L3" s="5">
+        <f t="shared" si="6"/>
         <v>502.9141902923584</v>
       </c>
-      <c r="M3" s="6">
-        <f>L3/1024</f>
+      <c r="M3" s="5">
+        <f t="shared" si="7"/>
         <v>0.49112713895738125</v>
       </c>
-      <c r="N3" s="6">
-        <f>L3/G3</f>
+      <c r="N3" s="5">
+        <f t="shared" si="8"/>
         <v>251.4570951461792</v>
       </c>
-      <c r="O3" s="6">
-        <f>N3/1024</f>
+      <c r="O3" s="5">
+        <f t="shared" si="9"/>
         <v>0.24556356947869062</v>
       </c>
       <c r="P3">
-        <f>G3*K3</f>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
     </row>
@@ -1167,61 +1163,61 @@
       <c r="A4">
         <v>60</v>
       </c>
-      <c r="B4" s="6">
-        <f>A4^4*8/2^30</f>
+      <c r="B4" s="5">
+        <f t="shared" si="0"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C4" s="6">
-        <f>4*B4</f>
+      <c r="C4" s="5">
+        <f t="shared" si="1"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D4" s="6">
-        <f>$D$2*(A4/$A$2)^6</f>
+      <c r="D4" s="5">
+        <f t="shared" si="11"/>
         <v>193.640625</v>
       </c>
-      <c r="E4" s="7">
-        <f>D4/60</f>
+      <c r="E4" s="5">
+        <f t="shared" si="2"/>
         <v>3.2273437500000002</v>
       </c>
-      <c r="F4" s="6">
-        <f>D4*100/(60*24)</f>
+      <c r="F4" s="5">
+        <f t="shared" si="3"/>
         <v>13.447265625</v>
       </c>
-      <c r="G4" s="6">
-        <f>CEILING(MAX(F4/3,1),1)</f>
+      <c r="G4" s="5">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>6</v>
       </c>
-      <c r="I4" s="6">
-        <f>H4*G4*B4</f>
+      <c r="I4" s="5">
+        <f t="shared" si="5"/>
         <v>2.8967857360839844</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>50</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>18</v>
       </c>
-      <c r="L4" s="6">
-        <f>I4*J4*K4</f>
+      <c r="L4" s="5">
+        <f t="shared" si="6"/>
         <v>2607.1071624755859</v>
       </c>
-      <c r="M4" s="6">
-        <f>L4/1024</f>
+      <c r="M4" s="5">
+        <f t="shared" si="7"/>
         <v>2.5460030883550644</v>
       </c>
-      <c r="N4" s="6">
-        <f>L4/G4</f>
+      <c r="N4" s="5">
+        <f t="shared" si="8"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O4" s="6">
-        <f>N4/1024</f>
+      <c r="O4" s="5">
+        <f t="shared" si="9"/>
         <v>0.50920061767101288</v>
       </c>
       <c r="P4">
-        <f>G4*K4</f>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
     </row>
@@ -1229,61 +1225,61 @@
       <c r="A5">
         <v>70</v>
       </c>
-      <c r="B5" s="6">
-        <f>A5^4*8/2^30</f>
+      <c r="B5" s="5">
+        <f t="shared" si="0"/>
         <v>0.17888844013214111</v>
       </c>
-      <c r="C5" s="6">
-        <f>4*B5</f>
+      <c r="C5" s="5">
+        <f t="shared" si="1"/>
         <v>0.71555376052856445</v>
       </c>
-      <c r="D5" s="6">
-        <f>$D$2*(A5/$A$2)^6</f>
+      <c r="D5" s="5">
+        <f t="shared" si="11"/>
         <v>488.289306640625</v>
       </c>
-      <c r="E5" s="7">
-        <f>D5/60</f>
+      <c r="E5" s="5">
+        <f t="shared" si="2"/>
         <v>8.1381551106770829</v>
       </c>
-      <c r="F5" s="6">
-        <f>D5*100/(60*24)</f>
+      <c r="F5" s="5">
+        <f t="shared" si="3"/>
         <v>33.908979627821182</v>
       </c>
-      <c r="G5" s="6">
-        <f>CEILING(MAX(F5/3,1),1)</f>
+      <c r="G5" s="5">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>6</v>
       </c>
-      <c r="I5" s="6">
-        <f>H5*G5*B5</f>
+      <c r="I5" s="5">
+        <f t="shared" si="5"/>
         <v>12.87996768951416</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>50</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>18</v>
       </c>
-      <c r="L5" s="6">
-        <f>I5*J5*K5</f>
+      <c r="L5" s="5">
+        <f t="shared" si="6"/>
         <v>11591.970920562744</v>
       </c>
-      <c r="M5" s="6">
-        <f>L5/1024</f>
+      <c r="M5" s="5">
+        <f t="shared" si="7"/>
         <v>11.320284102112055</v>
       </c>
-      <c r="N5" s="6">
-        <f>L5/G5</f>
+      <c r="N5" s="5">
+        <f t="shared" si="8"/>
         <v>965.99757671356201</v>
       </c>
-      <c r="O5" s="6">
-        <f>N5/1024</f>
+      <c r="O5" s="5">
+        <f t="shared" si="9"/>
         <v>0.9433570085093379</v>
       </c>
       <c r="P5">
-        <f>G5*K5</f>
+        <f t="shared" si="10"/>
         <v>216</v>
       </c>
     </row>
@@ -1291,61 +1287,61 @@
       <c r="A6">
         <v>80</v>
       </c>
-      <c r="B6" s="6">
-        <f>A6^4*8/2^30</f>
+      <c r="B6" s="5">
+        <f t="shared" si="0"/>
         <v>0.30517578125</v>
       </c>
-      <c r="C6" s="6">
-        <f>4*B6</f>
+      <c r="C6" s="5">
+        <f t="shared" si="1"/>
         <v>1.220703125</v>
       </c>
-      <c r="D6" s="6">
-        <f>$D$2*(A6/$A$2)^6</f>
+      <c r="D6" s="5">
+        <f t="shared" si="11"/>
         <v>1088</v>
       </c>
-      <c r="E6" s="7">
-        <f>D6/60</f>
+      <c r="E6" s="5">
+        <f t="shared" si="2"/>
         <v>18.133333333333333</v>
       </c>
-      <c r="F6" s="6">
-        <f>D6*100/(60*24)</f>
+      <c r="F6" s="5">
+        <f t="shared" si="3"/>
         <v>75.555555555555557</v>
       </c>
-      <c r="G6" s="6">
-        <f>CEILING(MAX(F6/3,1),1)</f>
+      <c r="G6" s="5">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>6</v>
       </c>
-      <c r="I6" s="6">
-        <f>H6*G6*B6</f>
+      <c r="I6" s="5">
+        <f t="shared" si="5"/>
         <v>47.607421875</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>50</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>18</v>
       </c>
-      <c r="L6" s="6">
-        <f>I6*J6*K6</f>
+      <c r="L6" s="5">
+        <f t="shared" si="6"/>
         <v>42846.6796875</v>
       </c>
-      <c r="M6" s="6">
-        <f>L6/1024</f>
+      <c r="M6" s="5">
+        <f t="shared" si="7"/>
         <v>41.842460632324219</v>
       </c>
-      <c r="N6" s="6">
-        <f>L6/G6</f>
+      <c r="N6" s="5">
+        <f t="shared" si="8"/>
         <v>1647.94921875</v>
       </c>
-      <c r="O6" s="6">
-        <f>N6/1024</f>
+      <c r="O6" s="5">
+        <f t="shared" si="9"/>
         <v>1.6093254089355469</v>
       </c>
       <c r="P6">
-        <f>G6*K6</f>
+        <f t="shared" si="10"/>
         <v>468</v>
       </c>
     </row>
@@ -1353,61 +1349,61 @@
       <c r="A7">
         <v>90</v>
       </c>
-      <c r="B7" s="6">
-        <f>A7^4*8/2^30</f>
+      <c r="B7" s="5">
+        <f t="shared" si="0"/>
         <v>0.48883259296417236</v>
       </c>
-      <c r="C7" s="6">
-        <f>4*B7</f>
+      <c r="C7" s="5">
+        <f t="shared" si="1"/>
         <v>1.9553303718566895</v>
       </c>
-      <c r="D7" s="6">
-        <f>$D$2*(A7/$A$2)^6</f>
+      <c r="D7" s="5">
+        <f t="shared" si="11"/>
         <v>2205.687744140625</v>
       </c>
-      <c r="E7" s="7">
-        <f>D7/60</f>
+      <c r="E7" s="5">
+        <f t="shared" si="2"/>
         <v>36.761462402343753</v>
       </c>
-      <c r="F7" s="6">
-        <f>D7*100/(60*24)</f>
+      <c r="F7" s="5">
+        <f t="shared" si="3"/>
         <v>153.17276000976562</v>
       </c>
-      <c r="G7" s="6">
-        <f>CEILING(MAX(F7/3,1),1)</f>
+      <c r="G7" s="5">
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>6</v>
       </c>
-      <c r="I7" s="6">
-        <f>H7*G7*B7</f>
+      <c r="I7" s="5">
+        <f t="shared" si="5"/>
         <v>152.51576900482178</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>50</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>18</v>
       </c>
-      <c r="L7" s="6">
-        <f>I7*J7*K7</f>
+      <c r="L7" s="5">
+        <f t="shared" si="6"/>
         <v>137264.1921043396</v>
       </c>
-      <c r="M7" s="6">
-        <f>L7/1024</f>
+      <c r="M7" s="5">
+        <f t="shared" si="7"/>
         <v>134.04706260189414</v>
       </c>
-      <c r="N7" s="6">
-        <f>L7/G7</f>
+      <c r="N7" s="5">
+        <f t="shared" si="8"/>
         <v>2639.6960020065308</v>
       </c>
-      <c r="O7" s="6">
-        <f>N7/1024</f>
+      <c r="O7" s="5">
+        <f t="shared" si="9"/>
         <v>2.5778281269595027</v>
       </c>
       <c r="P7">
-        <f>G7*K7</f>
+        <f t="shared" si="10"/>
         <v>936</v>
       </c>
     </row>
@@ -1415,61 +1411,61 @@
       <c r="A8">
         <v>100</v>
       </c>
-      <c r="B8" s="6">
-        <f>A8^4*8/2^30</f>
+      <c r="B8" s="5">
+        <f t="shared" si="0"/>
         <v>0.74505805969238281</v>
       </c>
-      <c r="C8" s="6">
-        <f>4*B8</f>
+      <c r="C8" s="5">
+        <f t="shared" si="1"/>
         <v>2.9802322387695312</v>
       </c>
-      <c r="D8" s="6">
-        <f>$D$2*(A8/$A$2)^6</f>
+      <c r="D8" s="5">
+        <f t="shared" si="11"/>
         <v>4150.390625</v>
       </c>
-      <c r="E8" s="7">
-        <f>D8/60</f>
+      <c r="E8" s="5">
+        <f t="shared" si="2"/>
         <v>69.173177083333329</v>
       </c>
-      <c r="F8" s="6">
-        <f>D8*100/(60*24)</f>
+      <c r="F8" s="5">
+        <f t="shared" si="3"/>
         <v>288.22157118055554</v>
       </c>
-      <c r="G8" s="6">
-        <f>CEILING(MAX(F8/3,1),1)</f>
+      <c r="G8" s="5">
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>6</v>
       </c>
-      <c r="I8" s="6">
-        <f>H8*G8*B8</f>
+      <c r="I8" s="5">
+        <f t="shared" si="5"/>
         <v>433.6237907409668</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>50</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>18</v>
       </c>
-      <c r="L8" s="6">
-        <f>I8*J8*K8</f>
+      <c r="L8" s="5">
+        <f t="shared" si="6"/>
         <v>390261.41166687012</v>
       </c>
-      <c r="M8" s="6">
-        <f>L8/1024</f>
+      <c r="M8" s="5">
+        <f t="shared" si="7"/>
         <v>381.11465983092785</v>
       </c>
-      <c r="N8" s="6">
-        <f>L8/G8</f>
+      <c r="N8" s="5">
+        <f t="shared" si="8"/>
         <v>4023.3135223388672</v>
       </c>
-      <c r="O8" s="6">
-        <f>N8/1024</f>
+      <c r="O8" s="5">
+        <f t="shared" si="9"/>
         <v>3.92901711165905</v>
       </c>
       <c r="P8">
-        <f>G8*K8</f>
+        <f t="shared" si="10"/>
         <v>1746</v>
       </c>
     </row>
@@ -1477,61 +1473,61 @@
       <c r="A9">
         <v>110</v>
       </c>
-      <c r="B9" s="6">
-        <f>A9^4*8/2^30</f>
+      <c r="B9" s="5">
+        <f t="shared" si="0"/>
         <v>1.0908395051956177</v>
       </c>
-      <c r="C9" s="6">
-        <f>4*B9</f>
+      <c r="C9" s="5">
+        <f t="shared" si="1"/>
         <v>4.3633580207824707</v>
       </c>
-      <c r="D9" s="6">
-        <f>$D$2*(A9/$A$2)^6</f>
+      <c r="D9" s="5">
+        <f t="shared" si="11"/>
         <v>7352.670166015625</v>
       </c>
-      <c r="E9" s="7">
-        <f>D9/60</f>
+      <c r="E9" s="5">
+        <f t="shared" si="2"/>
         <v>122.54450276692708</v>
       </c>
-      <c r="F9" s="6">
-        <f>D9*100/(60*24)</f>
+      <c r="F9" s="5">
+        <f t="shared" si="3"/>
         <v>510.60209486219617</v>
       </c>
-      <c r="G9" s="6">
-        <f>CEILING(MAX(F9/3,1),1)</f>
+      <c r="G9" s="5">
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>6</v>
       </c>
-      <c r="I9" s="6">
-        <f>H9*G9*B9</f>
+      <c r="I9" s="5">
+        <f t="shared" si="5"/>
         <v>1119.2013323307037</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>50</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>18</v>
       </c>
-      <c r="L9" s="6">
-        <f>I9*J9*K9</f>
+      <c r="L9" s="5">
+        <f t="shared" si="6"/>
         <v>1007281.1990976334</v>
       </c>
-      <c r="M9" s="6">
-        <f>L9/1024</f>
+      <c r="M9" s="5">
+        <f t="shared" si="7"/>
         <v>983.67304599378258</v>
       </c>
-      <c r="N9" s="6">
-        <f>L9/G9</f>
+      <c r="N9" s="5">
+        <f t="shared" si="8"/>
         <v>5890.5333280563354</v>
       </c>
-      <c r="O9" s="6">
-        <f>N9/1024</f>
+      <c r="O9" s="5">
+        <f t="shared" si="9"/>
         <v>5.7524739531800151</v>
       </c>
       <c r="P9">
-        <f>G9*K9</f>
+        <f t="shared" si="10"/>
         <v>3078</v>
       </c>
     </row>
@@ -1539,61 +1535,61 @@
       <c r="A10">
         <v>120</v>
       </c>
-      <c r="B10" s="6">
-        <f>A10^4*8/2^30</f>
+      <c r="B10" s="5">
+        <f t="shared" ref="B10:B15" si="12">A10^4*8/2^30</f>
         <v>1.544952392578125</v>
       </c>
-      <c r="C10" s="6">
-        <f>4*B10</f>
+      <c r="C10" s="5">
+        <f t="shared" ref="C10:C15" si="13">4*B10</f>
         <v>6.1798095703125</v>
       </c>
-      <c r="D10" s="6">
-        <f>$D$2*(A10/$A$2)^6</f>
+      <c r="D10" s="5">
+        <f t="shared" ref="D10:D15" si="14">$D$2*(A10/$A$2)^6</f>
         <v>12393</v>
       </c>
-      <c r="E10" s="7">
-        <f>D10/60</f>
+      <c r="E10" s="5">
+        <f t="shared" ref="E10:E15" si="15">D10/60</f>
         <v>206.55000000000001</v>
       </c>
-      <c r="F10" s="6">
-        <f>D10*100/(60*24)</f>
+      <c r="F10" s="5">
+        <f t="shared" ref="F10:F15" si="16">D10*100/(60*24)</f>
         <v>860.625</v>
       </c>
-      <c r="G10" s="6">
-        <f>CEILING(MAX(F10/3,1),1)</f>
+      <c r="G10" s="5">
+        <f t="shared" ref="G10:G15" si="17">CEILING(MAX(F10/3,1),1)</f>
         <v>287</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>6</v>
       </c>
-      <c r="I10" s="6">
-        <f>H10*G10*B10</f>
+      <c r="I10" s="5">
+        <f t="shared" ref="I10:I15" si="18">H10*G10*B10</f>
         <v>2660.4080200195312</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>50</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>18</v>
       </c>
-      <c r="L10" s="6">
-        <f>I10*J10*K10</f>
+      <c r="L10" s="5">
+        <f t="shared" ref="L10:L15" si="19">I10*J10*K10</f>
         <v>2394367.2180175781</v>
       </c>
-      <c r="M10" s="6">
-        <f>L10/1024</f>
+      <c r="M10" s="5">
+        <f t="shared" ref="M10:M15" si="20">L10/1024</f>
         <v>2338.2492363452911</v>
       </c>
-      <c r="N10" s="6">
-        <f>L10/G10</f>
+      <c r="N10" s="5">
+        <f t="shared" ref="N10:N15" si="21">L10/G10</f>
         <v>8342.742919921875</v>
       </c>
-      <c r="O10" s="6">
-        <f>N10/1024</f>
+      <c r="O10" s="5">
+        <f t="shared" ref="O10:O15" si="22">N10/1024</f>
         <v>8.1472098827362061</v>
       </c>
       <c r="P10">
-        <f>G10*K10</f>
+        <f t="shared" ref="P10:P15" si="23">G10*K10</f>
         <v>5166</v>
       </c>
     </row>
@@ -1601,61 +1597,61 @@
       <c r="A11">
         <v>130</v>
       </c>
-      <c r="B11" s="6">
-        <f>A11^4*8/2^30</f>
+      <c r="B11" s="5">
+        <f t="shared" si="12"/>
         <v>2.1279603242874146</v>
       </c>
-      <c r="C11" s="6">
-        <f>4*B11</f>
+      <c r="C11" s="5">
+        <f t="shared" si="13"/>
         <v>8.5118412971496582</v>
       </c>
-      <c r="D11" s="6">
-        <f>$D$2*(A11/$A$2)^6</f>
+      <c r="D11" s="5">
+        <f t="shared" si="14"/>
         <v>20033.142822265625</v>
       </c>
-      <c r="E11" s="7">
-        <f>D11/60</f>
+      <c r="E11" s="5">
+        <f t="shared" si="15"/>
         <v>333.88571370442708</v>
       </c>
-      <c r="F11" s="6">
-        <f>D11*100/(60*24)</f>
+      <c r="F11" s="5">
+        <f t="shared" si="16"/>
         <v>1391.1904737684463</v>
       </c>
-      <c r="G11" s="6">
-        <f>CEILING(MAX(F11/3,1),1)</f>
+      <c r="G11" s="5">
+        <f t="shared" si="17"/>
         <v>464</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>6</v>
       </c>
-      <c r="I11" s="6">
-        <f>H11*G11*B11</f>
+      <c r="I11" s="5">
+        <f t="shared" si="18"/>
         <v>5924.2415428161621</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>50</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>18</v>
       </c>
-      <c r="L11" s="6">
-        <f>I11*J11*K11</f>
+      <c r="L11" s="5">
+        <f t="shared" si="19"/>
         <v>5331817.3885345459</v>
       </c>
-      <c r="M11" s="6">
-        <f>L11/1024</f>
+      <c r="M11" s="5">
+        <f t="shared" si="20"/>
         <v>5206.8529184907675</v>
       </c>
-      <c r="N11" s="6">
-        <f>L11/G11</f>
+      <c r="N11" s="5">
+        <f t="shared" si="21"/>
         <v>11490.985751152039</v>
       </c>
-      <c r="O11" s="6">
-        <f>N11/1024</f>
+      <c r="O11" s="5">
+        <f t="shared" si="22"/>
         <v>11.221665772609413</v>
       </c>
       <c r="P11">
-        <f>G11*K11</f>
+        <f t="shared" si="23"/>
         <v>8352</v>
       </c>
     </row>
@@ -1663,61 +1659,61 @@
       <c r="A12">
         <v>140</v>
       </c>
-      <c r="B12" s="6">
-        <f>A12^4*8/2^30</f>
+      <c r="B12" s="5">
+        <f t="shared" si="12"/>
         <v>2.8622150421142578</v>
       </c>
-      <c r="C12" s="6">
-        <f>4*B12</f>
+      <c r="C12" s="5">
+        <f t="shared" si="13"/>
         <v>11.448860168457031</v>
       </c>
-      <c r="D12" s="6">
-        <f>$D$2*(A12/$A$2)^6</f>
+      <c r="D12" s="5">
+        <f t="shared" si="14"/>
         <v>31250.515625</v>
       </c>
-      <c r="E12" s="7">
-        <f>D12/60</f>
+      <c r="E12" s="5">
+        <f t="shared" si="15"/>
         <v>520.8419270833333</v>
       </c>
-      <c r="F12" s="6">
-        <f>D12*100/(60*24)</f>
+      <c r="F12" s="5">
+        <f t="shared" si="16"/>
         <v>2170.1746961805557</v>
       </c>
-      <c r="G12" s="6">
-        <f>CEILING(MAX(F12/3,1),1)</f>
+      <c r="G12" s="5">
+        <f t="shared" si="17"/>
         <v>724</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>6</v>
       </c>
-      <c r="I12" s="6">
-        <f>H12*G12*B12</f>
+      <c r="I12" s="5">
+        <f t="shared" si="18"/>
         <v>12433.462142944336</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>50</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>18</v>
       </c>
-      <c r="L12" s="6">
-        <f>I12*J12*K12</f>
+      <c r="L12" s="5">
+        <f t="shared" si="19"/>
         <v>11190115.928649902</v>
       </c>
-      <c r="M12" s="6">
-        <f>L12/1024</f>
+      <c r="M12" s="5">
+        <f t="shared" si="20"/>
         <v>10927.84758657217</v>
       </c>
-      <c r="N12" s="6">
-        <f>L12/G12</f>
+      <c r="N12" s="5">
+        <f t="shared" si="21"/>
         <v>15455.961227416992</v>
       </c>
-      <c r="O12" s="6">
-        <f>N12/1024</f>
+      <c r="O12" s="5">
+        <f t="shared" si="22"/>
         <v>15.093712136149406</v>
       </c>
       <c r="P12">
-        <f>G12*K12</f>
+        <f t="shared" si="23"/>
         <v>13032</v>
       </c>
     </row>
@@ -1725,61 +1721,61 @@
       <c r="A13">
         <v>150</v>
       </c>
-      <c r="B13" s="6">
-        <f>A13^4*8/2^30</f>
+      <c r="B13" s="5">
+        <f t="shared" si="12"/>
         <v>3.771856427192688</v>
       </c>
-      <c r="C13" s="6">
-        <f>4*B13</f>
+      <c r="C13" s="5">
+        <f t="shared" si="13"/>
         <v>15.087425708770752</v>
       </c>
-      <c r="D13" s="6">
-        <f>$D$2*(A13/$A$2)^6</f>
+      <c r="D13" s="5">
+        <f t="shared" si="14"/>
         <v>47275.543212890625</v>
       </c>
-      <c r="E13" s="7">
-        <f>D13/60</f>
+      <c r="E13" s="5">
+        <f t="shared" si="15"/>
         <v>787.92572021484375</v>
       </c>
-      <c r="F13" s="6">
-        <f>D13*100/(60*24)</f>
+      <c r="F13" s="5">
+        <f t="shared" si="16"/>
         <v>3283.0238342285156</v>
       </c>
-      <c r="G13" s="6">
-        <f>CEILING(MAX(F13/3,1),1)</f>
+      <c r="G13" s="5">
+        <f t="shared" si="17"/>
         <v>1095</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>6</v>
       </c>
-      <c r="I13" s="6">
-        <f>H13*G13*B13</f>
+      <c r="I13" s="5">
+        <f t="shared" si="18"/>
         <v>24781.09672665596</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>50</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>18</v>
       </c>
-      <c r="L13" s="6">
-        <f>I13*J13*K13</f>
+      <c r="L13" s="5">
+        <f t="shared" si="19"/>
         <v>22302987.053990364</v>
       </c>
-      <c r="M13" s="6">
-        <f>L13/1024</f>
+      <c r="M13" s="5">
+        <f t="shared" si="20"/>
         <v>21780.260794912465</v>
       </c>
-      <c r="N13" s="6">
-        <f>L13/G13</f>
+      <c r="N13" s="5">
+        <f t="shared" si="21"/>
         <v>20368.024706840515</v>
       </c>
-      <c r="O13" s="6">
-        <f>N13/1024</f>
+      <c r="O13" s="5">
+        <f t="shared" si="22"/>
         <v>19.890649127773941</v>
       </c>
       <c r="P13">
-        <f>G13*K13</f>
+        <f t="shared" si="23"/>
         <v>19710</v>
       </c>
     </row>
@@ -1787,61 +1783,61 @@
       <c r="A14">
         <v>76</v>
       </c>
-      <c r="B14" s="6">
-        <f>A14^4*8/2^30</f>
+      <c r="B14" s="5">
+        <f t="shared" si="12"/>
         <v>0.24856758117675781</v>
       </c>
-      <c r="C14" s="6">
-        <f>4*B14</f>
+      <c r="C14" s="5">
+        <f t="shared" si="13"/>
         <v>0.99427032470703125</v>
       </c>
-      <c r="D14" s="6">
-        <f>$D$2*(A14/$A$2)^6</f>
+      <c r="D14" s="5">
+        <f t="shared" si="14"/>
         <v>799.7799769999998</v>
       </c>
-      <c r="E14" s="6">
-        <f>D14/60</f>
+      <c r="E14" s="5">
+        <f t="shared" si="15"/>
         <v>13.32966628333333</v>
       </c>
-      <c r="F14" s="6">
-        <f>D14*100/(60*24)</f>
+      <c r="F14" s="5">
+        <f t="shared" si="16"/>
         <v>55.540276180555537</v>
       </c>
-      <c r="G14" s="6">
-        <f>CEILING(MAX(F14/3,1),1)</f>
+      <c r="G14" s="5">
+        <f t="shared" si="17"/>
         <v>19</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>6</v>
       </c>
-      <c r="I14" s="6">
-        <f>H14*G14*B14</f>
+      <c r="I14" s="5">
+        <f t="shared" si="18"/>
         <v>28.336704254150391</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>50</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>18</v>
       </c>
-      <c r="L14" s="6">
-        <f>I14*J14*K14</f>
+      <c r="L14" s="5">
+        <f t="shared" si="19"/>
         <v>25503.033828735352</v>
       </c>
-      <c r="M14" s="6">
-        <f>L14/1024</f>
+      <c r="M14" s="5">
+        <f t="shared" si="20"/>
         <v>24.905306473374367</v>
       </c>
-      <c r="N14" s="6">
-        <f>L14/G14</f>
+      <c r="N14" s="5">
+        <f t="shared" si="21"/>
         <v>1342.2649383544922</v>
       </c>
-      <c r="O14" s="6">
-        <f>N14/1024</f>
+      <c r="O14" s="5">
+        <f t="shared" si="22"/>
         <v>1.3108056038618088</v>
       </c>
       <c r="P14" s="2">
-        <f>G14*K14</f>
+        <f t="shared" si="23"/>
         <v>342</v>
       </c>
     </row>
@@ -1849,68 +1845,68 @@
       <c r="A15" s="2">
         <v>60</v>
       </c>
-      <c r="B15" s="6">
-        <f>A15^4*8/2^30</f>
+      <c r="B15" s="5">
+        <f t="shared" si="12"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C15" s="6">
-        <f>4*B15</f>
+      <c r="C15" s="5">
+        <f t="shared" si="13"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D15" s="6">
-        <f>$D$2*(A15/$A$2)^6</f>
+      <c r="D15" s="5">
+        <f t="shared" si="14"/>
         <v>193.640625</v>
       </c>
-      <c r="E15" s="6">
-        <f>D15/60</f>
+      <c r="E15" s="5">
+        <f t="shared" si="15"/>
         <v>3.2273437500000002</v>
       </c>
-      <c r="F15" s="6">
-        <f>D15*100/(60*24)</f>
+      <c r="F15" s="5">
+        <f t="shared" si="16"/>
         <v>13.447265625</v>
       </c>
-      <c r="G15" s="6">
-        <f>CEILING(MAX(F15/3,1),1)</f>
+      <c r="G15" s="5">
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>6</v>
       </c>
-      <c r="I15" s="6">
-        <f>H15*G15*B15</f>
+      <c r="I15" s="5">
+        <f t="shared" si="18"/>
         <v>2.8967857360839844</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>50</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>18</v>
       </c>
-      <c r="L15" s="6">
-        <f>I15*J15*K15</f>
+      <c r="L15" s="5">
+        <f t="shared" si="19"/>
         <v>2607.1071624755859</v>
       </c>
-      <c r="M15" s="6">
-        <f>L15/1024</f>
+      <c r="M15" s="5">
+        <f t="shared" si="20"/>
         <v>2.5460030883550644</v>
       </c>
-      <c r="N15" s="6">
-        <f>L15/G15</f>
+      <c r="N15" s="5">
+        <f t="shared" si="21"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O15" s="6">
-        <f>N15/1024</f>
+      <c r="O15" s="5">
+        <f t="shared" si="22"/>
         <v>0.50920061767101288</v>
       </c>
       <c r="P15" s="2">
-        <f>G15*K15</f>
+        <f t="shared" si="23"/>
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1922,7 +1918,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="15.140625"/>
     <col customWidth="1" min="3" max="3" width="12.8515625"/>
@@ -1942,7 +1938,7 @@
       <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1954,15 +1950,15 @@
         <v>17</v>
       </c>
       <c r="C2" s="3">
-        <f>B2/60</f>
+        <f t="shared" ref="C2:C9" si="24">B2/60</f>
         <v>0.28333333333333333</v>
       </c>
       <c r="D2" s="3">
-        <f>C2*100</f>
+        <f t="shared" ref="D2:D9" si="25">C2*100</f>
         <v>28.333333333333332</v>
       </c>
       <c r="E2" s="3">
-        <f>D2/24</f>
+        <f t="shared" ref="E2:E9" si="26">D2/24</f>
         <v>1.1805555555555556</v>
       </c>
     </row>
@@ -1971,19 +1967,19 @@
         <v>100</v>
       </c>
       <c r="B3" s="3">
-        <f>B2*(A3/A2)^6</f>
+        <f t="shared" ref="B3:B9" si="27">B2*(A3/A2)^6</f>
         <v>4150.390625</v>
       </c>
       <c r="C3" s="3">
-        <f>B3/60</f>
+        <f t="shared" si="24"/>
         <v>69.173177083333329</v>
       </c>
       <c r="D3" s="3">
-        <f>C3*100</f>
+        <f t="shared" si="25"/>
         <v>6917.317708333333</v>
       </c>
       <c r="E3" s="3">
-        <f>D3/24</f>
+        <f t="shared" si="26"/>
         <v>288.22157118055554</v>
       </c>
     </row>
@@ -1992,19 +1988,19 @@
         <v>50</v>
       </c>
       <c r="B4" s="3">
-        <f>B3*(A4/A3)^6</f>
+        <f t="shared" si="27"/>
         <v>64.849853515625</v>
       </c>
       <c r="C4" s="3">
-        <f>B4/60</f>
+        <f t="shared" si="24"/>
         <v>1.0808308919270833</v>
       </c>
       <c r="D4" s="3">
-        <f>C4*100</f>
+        <f t="shared" si="25"/>
         <v>108.08308919270833</v>
       </c>
       <c r="E4" s="3">
-        <f>D4/24</f>
+        <f t="shared" si="26"/>
         <v>4.5034620496961804</v>
       </c>
     </row>
@@ -2013,19 +2009,19 @@
         <v>60</v>
       </c>
       <c r="B5" s="3">
-        <f>B4*(A5/A4)^6</f>
+        <f t="shared" si="27"/>
         <v>193.64062499999994</v>
       </c>
       <c r="C5" s="3">
-        <f>B5/60</f>
+        <f t="shared" si="24"/>
         <v>3.2273437499999988</v>
       </c>
       <c r="D5" s="3">
-        <f>C5*100</f>
+        <f t="shared" si="25"/>
         <v>322.73437499999989</v>
       </c>
       <c r="E5" s="3">
-        <f>D5/24</f>
+        <f t="shared" si="26"/>
         <v>13.447265624999995</v>
       </c>
     </row>
@@ -2034,19 +2030,19 @@
         <v>70</v>
       </c>
       <c r="B6" s="3">
-        <f>B5*(A6/A5)^6</f>
+        <f t="shared" si="27"/>
         <v>488.28930664062506</v>
       </c>
       <c r="C6" s="3">
-        <f>B6/60</f>
+        <f t="shared" si="24"/>
         <v>8.1381551106770846</v>
       </c>
       <c r="D6" s="3">
-        <f>C6*100</f>
+        <f t="shared" si="25"/>
         <v>813.81551106770848</v>
       </c>
       <c r="E6" s="3">
-        <f>D6/24</f>
+        <f t="shared" si="26"/>
         <v>33.908979627821189</v>
       </c>
     </row>
@@ -2055,19 +2051,19 @@
         <v>80</v>
       </c>
       <c r="B7" s="3">
-        <f>B6*(A7/A6)^6</f>
+        <f t="shared" si="27"/>
         <v>1087.9999999999998</v>
       </c>
       <c r="C7" s="3">
-        <f>B7/60</f>
+        <f t="shared" si="24"/>
         <v>18.133333333333329</v>
       </c>
       <c r="D7" s="3">
-        <f>C7*100</f>
+        <f t="shared" si="25"/>
         <v>1813.333333333333</v>
       </c>
       <c r="E7" s="3">
-        <f>D7/24</f>
+        <f t="shared" si="26"/>
         <v>75.555555555555543</v>
       </c>
     </row>
@@ -2076,19 +2072,19 @@
         <v>90</v>
       </c>
       <c r="B8" s="3">
-        <f>B7*(A8/A7)^6</f>
+        <f t="shared" si="27"/>
         <v>2205.6877441406245</v>
       </c>
       <c r="C8" s="3">
-        <f>B8/60</f>
+        <f t="shared" si="24"/>
         <v>36.761462402343746</v>
       </c>
       <c r="D8" s="3">
-        <f>C8*100</f>
+        <f t="shared" si="25"/>
         <v>3676.1462402343745</v>
       </c>
       <c r="E8" s="3">
-        <f>D8/24</f>
+        <f t="shared" si="26"/>
         <v>153.1727600097656</v>
       </c>
     </row>
@@ -2097,19 +2093,19 @@
         <v>100</v>
       </c>
       <c r="B9" s="3">
-        <f>B8*(A9/A8)^6</f>
+        <f t="shared" si="27"/>
         <v>4150.390625</v>
       </c>
       <c r="C9" s="3">
-        <f>B9/60</f>
+        <f t="shared" si="24"/>
         <v>69.173177083333329</v>
       </c>
       <c r="D9" s="3">
-        <f>C9*100</f>
+        <f t="shared" si="25"/>
         <v>6917.317708333333</v>
       </c>
       <c r="E9" s="3">
-        <f>D9/24</f>
+        <f t="shared" si="26"/>
         <v>288.22157118055554</v>
       </c>
     </row>
@@ -2122,15 +2118,15 @@
         <v>7352.6701660156286</v>
       </c>
       <c r="C10" s="3">
-        <f>B10/60</f>
+        <f t="shared" ref="C10:C11" si="28">B10/60</f>
         <v>122.54450276692714</v>
       </c>
       <c r="D10" s="3">
-        <f>C10*100</f>
+        <f t="shared" ref="D10:D11" si="29">C10*100</f>
         <v>12254.450276692714</v>
       </c>
       <c r="E10" s="3">
-        <f>D10/24</f>
+        <f t="shared" ref="E10:E11" si="30">D10/24</f>
         <v>510.60209486219645</v>
       </c>
     </row>
@@ -2143,15 +2139,15 @@
         <v>12393</v>
       </c>
       <c r="C11" s="3">
-        <f>B11/60</f>
+        <f t="shared" si="28"/>
         <v>206.55000000000001</v>
       </c>
       <c r="D11" s="3">
-        <f>C11*100</f>
+        <f t="shared" si="29"/>
         <v>20655</v>
       </c>
       <c r="E11" s="3">
-        <f>D11/24</f>
+        <f t="shared" si="30"/>
         <v>860.625</v>
       </c>
     </row>
@@ -2159,7 +2155,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2356,7 +2352,7 @@
         <v>2</v>
       </c>
       <c r="H21">
-        <f>SUM(A21:G21)</f>
+        <f t="shared" ref="H21:H24" si="31">SUM(A21:G21)</f>
         <v>16</v>
       </c>
     </row>
@@ -2377,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <f>SUM(A22:G22)</f>
+        <f t="shared" si="31"/>
         <v>16</v>
       </c>
     </row>
@@ -2395,7 +2391,7 @@
         <v>4</v>
       </c>
       <c r="H23">
-        <f>SUM(A23:G23)</f>
+        <f t="shared" si="31"/>
         <v>24</v>
       </c>
     </row>
@@ -2416,7 +2412,7 @@
         <v>2</v>
       </c>
       <c r="H24">
-        <f>SUM(A24:G24)</f>
+        <f t="shared" si="31"/>
         <v>18</v>
       </c>
     </row>
@@ -2427,6 +2423,26 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Added program to calculate the keldysh green's function values. Added notebooks for visualizing the initial condition and particle densities.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -974,7 +974,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -2435,7 +2435,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="7"/>
     <row r="8"/>
@@ -2443,7 +2443,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new executable for running without energy binning. Added notebooks for visualizing imbalance and energy distributions.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -1049,15 +1050,15 @@
         <v>0.0762939453125</v>
       </c>
       <c r="D2" s="5">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E2" s="5">
         <f t="shared" ref="E2:E9" si="2">D2/60</f>
-        <v>0.28333333333333333</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F9" si="3">D2*100/(60*24)</f>
-        <v>1.1805555555555556</v>
+        <v>2.2916666666666665</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G9" si="4">CEILING(MAX(F2/3,1),1)</f>
@@ -1111,26 +1112,26 @@
       </c>
       <c r="D3" s="5">
         <f t="shared" ref="D3:D9" si="11">$D$2*(A3/$A$2)^6</f>
-        <v>64.849853515625</v>
+        <v>125.885009765625</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" si="2"/>
-        <v>1.0808308919270833</v>
+        <v>2.09808349609375</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="3"/>
-        <v>4.5034620496961804</v>
+        <v>8.7420145670572911</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="5">
         <v>6</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="5"/>
-        <v>0.55879354476928711</v>
+        <v>0.83819031715393066</v>
       </c>
       <c r="J3" s="5">
         <v>50</v>
@@ -1140,11 +1141,11 @@
       </c>
       <c r="L3" s="5">
         <f t="shared" si="6"/>
-        <v>502.9141902923584</v>
+        <v>754.3712854385376</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" si="7"/>
-        <v>0.49112713895738125</v>
+        <v>0.73669070843607187</v>
       </c>
       <c r="N3" s="5">
         <f t="shared" si="8"/>
@@ -1156,7 +1157,7 @@
       </c>
       <c r="P3">
         <f t="shared" si="10"/>
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" ht="14.25">
@@ -1173,26 +1174,26 @@
       </c>
       <c r="D4" s="5">
         <f t="shared" si="11"/>
-        <v>193.640625</v>
+        <v>375.890625</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="2"/>
-        <v>3.2273437500000002</v>
+        <v>6.2648437499999998</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="3"/>
-        <v>13.447265625</v>
+        <v>26.103515625</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H4" s="5">
         <v>6</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="5"/>
-        <v>2.8967857360839844</v>
+        <v>5.2142143249511719</v>
       </c>
       <c r="J4" s="5">
         <v>50</v>
@@ -1202,11 +1203,11 @@
       </c>
       <c r="L4" s="5">
         <f t="shared" si="6"/>
-        <v>2607.1071624755859</v>
+        <v>4692.7928924560547</v>
       </c>
       <c r="M4" s="5">
         <f t="shared" si="7"/>
-        <v>2.5460030883550644</v>
+        <v>4.5828055590391159</v>
       </c>
       <c r="N4" s="5">
         <f t="shared" si="8"/>
@@ -1218,7 +1219,7 @@
       </c>
       <c r="P4">
         <f t="shared" si="10"/>
-        <v>90</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1235,26 +1236,26 @@
       </c>
       <c r="D5" s="5">
         <f t="shared" si="11"/>
-        <v>488.289306640625</v>
+        <v>947.855712890625</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="2"/>
-        <v>8.1381551106770829</v>
+        <v>15.797595214843749</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="3"/>
-        <v>33.908979627821182</v>
+        <v>65.823313395182296</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H5" s="5">
         <v>6</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="5"/>
-        <v>12.87996768951416</v>
+        <v>23.613274097442627</v>
       </c>
       <c r="J5" s="5">
         <v>50</v>
@@ -1264,11 +1265,11 @@
       </c>
       <c r="L5" s="5">
         <f t="shared" si="6"/>
-        <v>11591.970920562744</v>
+        <v>21251.946687698364</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" si="7"/>
-        <v>11.320284102112055</v>
+        <v>20.753854187205434</v>
       </c>
       <c r="N5" s="5">
         <f t="shared" si="8"/>
@@ -1280,7 +1281,7 @@
       </c>
       <c r="P5">
         <f t="shared" si="10"/>
-        <v>216</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -1297,26 +1298,26 @@
       </c>
       <c r="D6" s="5">
         <f t="shared" si="11"/>
-        <v>1088</v>
+        <v>2112</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="2"/>
-        <v>18.133333333333333</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="3"/>
-        <v>75.555555555555557</v>
+        <v>146.66666666666666</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="H6" s="5">
         <v>6</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="5"/>
-        <v>47.607421875</v>
+        <v>89.7216796875</v>
       </c>
       <c r="J6" s="5">
         <v>50</v>
@@ -1326,11 +1327,11 @@
       </c>
       <c r="L6" s="5">
         <f t="shared" si="6"/>
-        <v>42846.6796875</v>
+        <v>80749.51171875</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="7"/>
-        <v>41.842460632324219</v>
+        <v>78.856945037841797</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="8"/>
@@ -1342,7 +1343,7 @@
       </c>
       <c r="P6">
         <f t="shared" si="10"/>
-        <v>468</v>
+        <v>882</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1359,26 +1360,26 @@
       </c>
       <c r="D7" s="5">
         <f t="shared" si="11"/>
-        <v>2205.687744140625</v>
+        <v>4281.629150390625</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="2"/>
-        <v>36.761462402343753</v>
+        <v>71.360485839843747</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="3"/>
-        <v>153.17276000976562</v>
+        <v>297.33535766601562</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="H7" s="5">
         <v>6</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="5"/>
-        <v>152.51576900482178</v>
+        <v>293.29955577850342</v>
       </c>
       <c r="J7" s="5">
         <v>50</v>
@@ -1388,11 +1389,11 @@
       </c>
       <c r="L7" s="5">
         <f t="shared" si="6"/>
-        <v>137264.1921043396</v>
+        <v>263969.60020065308</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="7"/>
-        <v>134.04706260189414</v>
+        <v>257.78281269595027</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="8"/>
@@ -1404,7 +1405,7 @@
       </c>
       <c r="P7">
         <f t="shared" si="10"/>
-        <v>936</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="8" ht="14.25">
@@ -1421,52 +1422,52 @@
       </c>
       <c r="D8" s="5">
         <f t="shared" si="11"/>
-        <v>4150.390625</v>
+        <v>8056.640625</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="2"/>
-        <v>69.173177083333329</v>
+        <v>134.27734375</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="3"/>
-        <v>288.22157118055554</v>
+        <v>559.48893229166663</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="4"/>
-        <v>97</v>
+        <v>187</v>
       </c>
       <c r="H8" s="5">
         <v>6</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="5"/>
-        <v>433.6237907409668</v>
+        <v>835.95514297485352</v>
       </c>
       <c r="J8" s="5">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="K8" s="5">
-        <v>18</v>
+        <v>231</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="6"/>
-        <v>390261.41166687012</v>
+        <v>193105.63802719116</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="7"/>
-        <v>381.11465983092785</v>
+        <v>188.57972463592887</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="8"/>
-        <v>4023.3135223388672</v>
+        <v>1032.6504707336426</v>
       </c>
       <c r="O8" s="5">
         <f t="shared" si="9"/>
-        <v>3.92901711165905</v>
+        <v>1.0084477253258228</v>
       </c>
       <c r="P8">
         <f t="shared" si="10"/>
-        <v>1746</v>
+        <v>43197</v>
       </c>
     </row>
     <row r="9" ht="14.25">
@@ -1483,26 +1484,26 @@
       </c>
       <c r="D9" s="5">
         <f t="shared" si="11"/>
-        <v>7352.670166015625</v>
+        <v>14272.830322265625</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="2"/>
-        <v>122.54450276692708</v>
+        <v>237.88050537109376</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="3"/>
-        <v>510.60209486219617</v>
+        <v>991.16877237955725</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="4"/>
-        <v>171</v>
+        <v>331</v>
       </c>
       <c r="H9" s="5">
         <v>6</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>1119.2013323307037</v>
+        <v>2166.4072573184967</v>
       </c>
       <c r="J9" s="5">
         <v>50</v>
@@ -1512,11 +1513,11 @@
       </c>
       <c r="L9" s="5">
         <f t="shared" si="6"/>
-        <v>1007281.1990976334</v>
+        <v>1949766.531586647</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="7"/>
-        <v>983.67304599378258</v>
+        <v>1904.068878502585</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" si="8"/>
@@ -1528,7 +1529,7 @@
       </c>
       <c r="P9">
         <f t="shared" si="10"/>
-        <v>3078</v>
+        <v>5958</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -1545,26 +1546,26 @@
       </c>
       <c r="D10" s="5">
         <f t="shared" ref="D10:D15" si="14">$D$2*(A10/$A$2)^6</f>
-        <v>12393</v>
+        <v>24057</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" ref="E10:E15" si="15">D10/60</f>
-        <v>206.55000000000001</v>
+        <v>400.94999999999999</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ref="F10:F15" si="16">D10*100/(60*24)</f>
-        <v>860.625</v>
+        <v>1670.625</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" ref="G10:G15" si="17">CEILING(MAX(F10/3,1),1)</f>
-        <v>287</v>
+        <v>557</v>
       </c>
       <c r="H10" s="5">
         <v>6</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" ref="I10:I15" si="18">H10*G10*B10</f>
-        <v>2660.4080200195312</v>
+        <v>5163.2308959960938</v>
       </c>
       <c r="J10" s="5">
         <v>50</v>
@@ -1574,11 +1575,11 @@
       </c>
       <c r="L10" s="5">
         <f t="shared" ref="L10:L15" si="19">I10*J10*K10</f>
-        <v>2394367.2180175781</v>
+        <v>4646907.8063964844</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" ref="M10:M15" si="20">L10/1024</f>
-        <v>2338.2492363452911</v>
+        <v>4537.9959046840668</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" ref="N10:N15" si="21">L10/G10</f>
@@ -1590,7 +1591,7 @@
       </c>
       <c r="P10">
         <f t="shared" ref="P10:P15" si="23">G10*K10</f>
-        <v>5166</v>
+        <v>10026</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -1607,26 +1608,26 @@
       </c>
       <c r="D11" s="5">
         <f t="shared" si="14"/>
-        <v>20033.142822265625</v>
+        <v>38887.865478515625</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="15"/>
-        <v>333.88571370442708</v>
+        <v>648.1310913085938</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="16"/>
-        <v>1391.1904737684463</v>
+        <v>2700.5462137858071</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="17"/>
-        <v>464</v>
+        <v>901</v>
       </c>
       <c r="H11" s="5">
         <v>6</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="18"/>
-        <v>5924.2415428161621</v>
+        <v>11503.753513097763</v>
       </c>
       <c r="J11" s="5">
         <v>50</v>
@@ -1636,11 +1637,11 @@
       </c>
       <c r="L11" s="5">
         <f t="shared" si="19"/>
-        <v>5331817.3885345459</v>
+        <v>10353378.161787987</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="20"/>
-        <v>5206.8529184907675</v>
+        <v>10110.720861121081</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="21"/>
@@ -1652,7 +1653,7 @@
       </c>
       <c r="P11">
         <f t="shared" si="23"/>
-        <v>8352</v>
+        <v>16218</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -1669,26 +1670,26 @@
       </c>
       <c r="D12" s="5">
         <f t="shared" si="14"/>
-        <v>31250.515625</v>
+        <v>60662.765625</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="15"/>
-        <v>520.8419270833333</v>
+        <v>1011.04609375</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="16"/>
-        <v>2170.1746961805557</v>
+        <v>4212.692057291667</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="17"/>
-        <v>724</v>
+        <v>1405</v>
       </c>
       <c r="H12" s="5">
         <v>6</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="18"/>
-        <v>12433.462142944336</v>
+        <v>24128.472805023193</v>
       </c>
       <c r="J12" s="5">
         <v>50</v>
@@ -1698,11 +1699,11 @@
       </c>
       <c r="L12" s="5">
         <f t="shared" si="19"/>
-        <v>11190115.928649902</v>
+        <v>21715625.524520874</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="20"/>
-        <v>10927.84758657217</v>
+        <v>21206.665551289916</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" si="21"/>
@@ -1714,7 +1715,7 @@
       </c>
       <c r="P12">
         <f t="shared" si="23"/>
-        <v>13032</v>
+        <v>25290</v>
       </c>
     </row>
     <row r="13" ht="14.25">
@@ -1731,26 +1732,26 @@
       </c>
       <c r="D13" s="5">
         <f t="shared" si="14"/>
-        <v>47275.543212890625</v>
+        <v>91770.172119140625</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="15"/>
-        <v>787.92572021484375</v>
+        <v>1529.5028686523438</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="16"/>
-        <v>3283.0238342285156</v>
+        <v>6372.9286193847656</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="17"/>
-        <v>1095</v>
+        <v>2125</v>
       </c>
       <c r="H13" s="5">
         <v>6</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="18"/>
-        <v>24781.09672665596</v>
+        <v>48091.169446706772</v>
       </c>
       <c r="J13" s="5">
         <v>50</v>
@@ -1760,11 +1761,11 @@
       </c>
       <c r="L13" s="5">
         <f t="shared" si="19"/>
-        <v>22302987.053990364</v>
+        <v>43282052.502036095</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="20"/>
-        <v>21780.260794912465</v>
+        <v>42267.629396519624</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="21"/>
@@ -1776,7 +1777,7 @@
       </c>
       <c r="P13">
         <f t="shared" si="23"/>
-        <v>19710</v>
+        <v>38250</v>
       </c>
     </row>
     <row r="14" ht="14.25">
@@ -1793,26 +1794,26 @@
       </c>
       <c r="D14" s="5">
         <f t="shared" si="14"/>
-        <v>799.7799769999998</v>
+        <v>1552.5140729999996</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="15"/>
-        <v>13.32966628333333</v>
+        <v>25.875234549999995</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="16"/>
-        <v>55.540276180555537</v>
+        <v>107.81347729166664</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="17"/>
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H14" s="5">
         <v>6</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="18"/>
-        <v>28.336704254150391</v>
+        <v>53.690597534179688</v>
       </c>
       <c r="J14" s="5">
         <v>50</v>
@@ -1822,11 +1823,11 @@
       </c>
       <c r="L14" s="5">
         <f t="shared" si="19"/>
-        <v>25503.033828735352</v>
+        <v>48321.537780761719</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="20"/>
-        <v>24.905306473374367</v>
+        <v>47.189001739025116</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="21"/>
@@ -1838,7 +1839,7 @@
       </c>
       <c r="P14" s="2">
         <f t="shared" si="23"/>
-        <v>342</v>
+        <v>648</v>
       </c>
     </row>
     <row r="15" ht="14.25">
@@ -1855,26 +1856,26 @@
       </c>
       <c r="D15" s="5">
         <f t="shared" si="14"/>
-        <v>193.640625</v>
+        <v>375.890625</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="15"/>
-        <v>3.2273437500000002</v>
+        <v>6.2648437499999998</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="16"/>
-        <v>13.447265625</v>
+        <v>26.103515625</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="17"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H15" s="5">
         <v>6</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="18"/>
-        <v>2.8967857360839844</v>
+        <v>5.2142143249511719</v>
       </c>
       <c r="J15" s="5">
         <v>50</v>
@@ -1884,11 +1885,11 @@
       </c>
       <c r="L15" s="5">
         <f t="shared" si="19"/>
-        <v>2607.1071624755859</v>
+        <v>4692.7928924560547</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="20"/>
-        <v>2.5460030883550644</v>
+        <v>4.5828055590391159</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="21"/>
@@ -1900,7 +1901,7 @@
       </c>
       <c r="P15" s="2">
         <f t="shared" si="23"/>
-        <v>90</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1912,6 +1913,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1">
+        <f>24*3*60</f>
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <f>1100/50</f>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
@@ -2160,7 +2190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
@@ -2428,7 +2458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">

</xml_diff>

<commit_message>
Changed output format to binary. Also changed keldysh_window_batch to only write to a file every 5 realizations or at the last run.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>L</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">For 24 L^2 Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For 28 L^2 Size</t>
   </si>
   <si>
     <t xml:space="preserve">Real Size L^2xL^2 (in GB)</t>
@@ -166,13 +169,19 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -915,7 +924,29 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="F12" s="2"/>
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <f>(28/4)*B7</f>
+        <v>20.861625671386719</v>
+      </c>
+      <c r="C12" s="5">
+        <f>(28/4)*C7</f>
+        <v>0.5340576171875</v>
+      </c>
+      <c r="D12" s="5">
+        <f>(28/4)*D7</f>
+        <v>13.687312602996826</v>
+      </c>
+      <c r="E12" s="5">
+        <f>(28/4)*E7</f>
+        <v>8.544921875</v>
+      </c>
+      <c r="F12" s="5">
+        <f>(28/4)*F7</f>
+        <v>2.7036666870117188</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
       <c r="F13" s="2"/>
@@ -987,109 +1018,109 @@
     <col bestFit="1" min="13" max="14" width="9.4609375"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="85.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="6" customFormat="1" ht="85.5">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>23</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
         <v>40</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <f t="shared" ref="B2:B9" si="0">A2^4*8/2^30</f>
         <v>0.019073486328125</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="7">
         <f t="shared" ref="C2:C9" si="1">4*B2</f>
         <v>0.0762939453125</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="7">
         <v>33</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="7">
         <f t="shared" ref="E2:E9" si="2">D2/60</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="7">
         <f t="shared" ref="F2:F9" si="3">D2*100/(60*24)</f>
         <v>2.2916666666666665</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="7">
         <f t="shared" ref="G2:G9" si="4">CEILING(MAX(F2/3,1),1)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="7">
         <v>6</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="7">
         <f t="shared" ref="I2:I9" si="5">H2*G2*B2</f>
         <v>0.11444091796875</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="7">
         <v>50</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="7">
         <v>18</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="7">
         <f t="shared" ref="L2:L9" si="6">I2*J2*K2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="7">
         <f t="shared" ref="M2:M9" si="7">L2/1024</f>
         <v>0.10058283805847168</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="7">
         <f t="shared" ref="N2:N9" si="8">L2/G2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="7">
         <f t="shared" ref="O2:O9" si="9">N2/1024</f>
         <v>0.10058283805847168</v>
       </c>
@@ -1102,56 +1133,56 @@
       <c r="A3">
         <v>50</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <f t="shared" si="0"/>
         <v>0.046566128730773926</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="7">
         <f t="shared" si="1"/>
         <v>0.1862645149230957</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="7">
         <f t="shared" ref="D3:D9" si="11">$D$2*(A3/$A$2)^6</f>
         <v>125.885009765625</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="7">
         <f t="shared" si="2"/>
         <v>2.09808349609375</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="7">
         <f t="shared" si="3"/>
         <v>8.7420145670572911</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="7">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="7">
         <v>6</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="7">
         <f t="shared" si="5"/>
         <v>0.83819031715393066</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="7">
         <v>50</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="7">
         <v>18</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="7">
         <f t="shared" si="6"/>
         <v>754.3712854385376</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="7">
         <f t="shared" si="7"/>
         <v>0.73669070843607187</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="7">
         <f t="shared" si="8"/>
         <v>251.4570951461792</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="7">
         <f t="shared" si="9"/>
         <v>0.24556356947869062</v>
       </c>
@@ -1164,56 +1195,56 @@
       <c r="A4">
         <v>60</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="7">
         <f t="shared" si="0"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="7">
         <f t="shared" si="1"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="7">
         <f t="shared" si="11"/>
         <v>375.890625</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="7">
         <f t="shared" si="2"/>
         <v>6.2648437499999998</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="7">
         <f t="shared" si="3"/>
         <v>26.103515625</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="7">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="7">
         <v>6</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="7">
         <f t="shared" si="5"/>
         <v>5.2142143249511719</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="7">
         <v>50</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="7">
         <v>18</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="7">
         <f t="shared" si="6"/>
         <v>4692.7928924560547</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="7">
         <f t="shared" si="7"/>
         <v>4.5828055590391159</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="7">
         <f t="shared" si="8"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="7">
         <f t="shared" si="9"/>
         <v>0.50920061767101288</v>
       </c>
@@ -1226,56 +1257,56 @@
       <c r="A5">
         <v>70</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <f t="shared" si="0"/>
         <v>0.17888844013214111</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="7">
         <f t="shared" si="1"/>
         <v>0.71555376052856445</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="7">
         <f t="shared" si="11"/>
         <v>947.855712890625</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="7">
         <f t="shared" si="2"/>
         <v>15.797595214843749</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="7">
         <f t="shared" si="3"/>
         <v>65.823313395182296</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="7">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="7">
         <v>6</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="7">
         <f t="shared" si="5"/>
         <v>23.613274097442627</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="7">
         <v>50</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="7">
         <v>18</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="7">
         <f t="shared" si="6"/>
         <v>21251.946687698364</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="7">
         <f t="shared" si="7"/>
         <v>20.753854187205434</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="7">
         <f t="shared" si="8"/>
         <v>965.99757671356201</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="7">
         <f t="shared" si="9"/>
         <v>0.9433570085093379</v>
       </c>
@@ -1288,56 +1319,56 @@
       <c r="A6">
         <v>80</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="7">
         <f t="shared" si="0"/>
         <v>0.30517578125</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="7">
         <f t="shared" si="1"/>
         <v>1.220703125</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="7">
         <f t="shared" si="11"/>
         <v>2112</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="7">
         <f t="shared" si="2"/>
         <v>35.200000000000003</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="7">
         <f t="shared" si="3"/>
         <v>146.66666666666666</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="7">
         <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="7">
         <v>6</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="7">
         <f t="shared" si="5"/>
         <v>89.7216796875</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="7">
         <v>50</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="7">
         <v>18</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="7">
         <f t="shared" si="6"/>
         <v>80749.51171875</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="7">
         <f t="shared" si="7"/>
         <v>78.856945037841797</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="7">
         <f t="shared" si="8"/>
         <v>1647.94921875</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="7">
         <f t="shared" si="9"/>
         <v>1.6093254089355469</v>
       </c>
@@ -1350,56 +1381,56 @@
       <c r="A7">
         <v>90</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="7">
         <f t="shared" si="0"/>
         <v>0.48883259296417236</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="7">
         <f t="shared" si="1"/>
         <v>1.9553303718566895</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="7">
         <f t="shared" si="11"/>
         <v>4281.629150390625</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="7">
         <f t="shared" si="2"/>
         <v>71.360485839843747</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="7">
         <f t="shared" si="3"/>
         <v>297.33535766601562</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="7">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="7">
         <v>6</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="7">
         <f t="shared" si="5"/>
         <v>293.29955577850342</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="7">
         <v>50</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="7">
         <v>18</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="7">
         <f t="shared" si="6"/>
         <v>263969.60020065308</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="7">
         <f t="shared" si="7"/>
         <v>257.78281269595027</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="7">
         <f t="shared" si="8"/>
         <v>2639.6960020065308</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="7">
         <f t="shared" si="9"/>
         <v>2.5778281269595027</v>
       </c>
@@ -1412,56 +1443,56 @@
       <c r="A8">
         <v>100</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <f t="shared" si="0"/>
         <v>0.74505805969238281</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="7">
         <f t="shared" si="1"/>
         <v>2.9802322387695312</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="7">
         <f t="shared" si="11"/>
         <v>8056.640625</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="7">
         <f t="shared" si="2"/>
         <v>134.27734375</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="7">
         <f t="shared" si="3"/>
         <v>559.48893229166663</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="7">
         <f t="shared" si="4"/>
         <v>187</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="7">
         <v>6</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="7">
         <f t="shared" si="5"/>
         <v>835.95514297485352</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="7">
         <v>1</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="7">
         <v>231</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="7">
         <f t="shared" si="6"/>
         <v>193105.63802719116</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="7">
         <f t="shared" si="7"/>
         <v>188.57972463592887</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="7">
         <f t="shared" si="8"/>
         <v>1032.6504707336426</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="7">
         <f t="shared" si="9"/>
         <v>1.0084477253258228</v>
       </c>
@@ -1474,56 +1505,56 @@
       <c r="A9">
         <v>110</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="7">
         <f t="shared" si="0"/>
         <v>1.0908395051956177</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="7">
         <f t="shared" si="1"/>
         <v>4.3633580207824707</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="7">
         <f t="shared" si="11"/>
         <v>14272.830322265625</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="7">
         <f t="shared" si="2"/>
         <v>237.88050537109376</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="7">
         <f t="shared" si="3"/>
         <v>991.16877237955725</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="7">
         <f t="shared" si="4"/>
         <v>331</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="7">
         <v>6</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="7">
         <f t="shared" si="5"/>
         <v>2166.4072573184967</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="7">
         <v>50</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="7">
         <v>18</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="7">
         <f t="shared" si="6"/>
         <v>1949766.531586647</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="7">
         <f t="shared" si="7"/>
         <v>1904.068878502585</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="7">
         <f t="shared" si="8"/>
         <v>5890.5333280563354</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="7">
         <f t="shared" si="9"/>
         <v>5.7524739531800151</v>
       </c>
@@ -1536,56 +1567,56 @@
       <c r="A10">
         <v>120</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="7">
         <f t="shared" ref="B10:B15" si="12">A10^4*8/2^30</f>
         <v>1.544952392578125</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="7">
         <f t="shared" ref="C10:C15" si="13">4*B10</f>
         <v>6.1798095703125</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="7">
         <f t="shared" ref="D10:D15" si="14">$D$2*(A10/$A$2)^6</f>
         <v>24057</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="7">
         <f t="shared" ref="E10:E15" si="15">D10/60</f>
         <v>400.94999999999999</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="7">
         <f t="shared" ref="F10:F15" si="16">D10*100/(60*24)</f>
         <v>1670.625</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="7">
         <f t="shared" ref="G10:G15" si="17">CEILING(MAX(F10/3,1),1)</f>
         <v>557</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="7">
         <v>6</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="7">
         <f t="shared" ref="I10:I15" si="18">H10*G10*B10</f>
         <v>5163.2308959960938</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="7">
         <v>50</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="7">
         <v>18</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="7">
         <f t="shared" ref="L10:L15" si="19">I10*J10*K10</f>
         <v>4646907.8063964844</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="7">
         <f t="shared" ref="M10:M15" si="20">L10/1024</f>
         <v>4537.9959046840668</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="7">
         <f t="shared" ref="N10:N15" si="21">L10/G10</f>
         <v>8342.742919921875</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="7">
         <f t="shared" ref="O10:O15" si="22">N10/1024</f>
         <v>8.1472098827362061</v>
       </c>
@@ -1598,56 +1629,56 @@
       <c r="A11">
         <v>130</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="7">
         <f t="shared" si="12"/>
         <v>2.1279603242874146</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="7">
         <f t="shared" si="13"/>
         <v>8.5118412971496582</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="7">
         <f t="shared" si="14"/>
         <v>38887.865478515625</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="7">
         <f t="shared" si="15"/>
         <v>648.1310913085938</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="7">
         <f t="shared" si="16"/>
         <v>2700.5462137858071</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="7">
         <f t="shared" si="17"/>
         <v>901</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="7">
         <v>6</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="7">
         <f t="shared" si="18"/>
         <v>11503.753513097763</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="7">
         <v>50</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="7">
         <v>18</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="7">
         <f t="shared" si="19"/>
         <v>10353378.161787987</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="7">
         <f t="shared" si="20"/>
         <v>10110.720861121081</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="7">
         <f t="shared" si="21"/>
         <v>11490.985751152039</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="7">
         <f t="shared" si="22"/>
         <v>11.221665772609413</v>
       </c>
@@ -1660,56 +1691,56 @@
       <c r="A12">
         <v>140</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="7">
         <f t="shared" si="12"/>
         <v>2.8622150421142578</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="7">
         <f t="shared" si="13"/>
         <v>11.448860168457031</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="7">
         <f t="shared" si="14"/>
         <v>60662.765625</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="7">
         <f t="shared" si="15"/>
         <v>1011.04609375</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="7">
         <f t="shared" si="16"/>
         <v>4212.692057291667</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="7">
         <f t="shared" si="17"/>
         <v>1405</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="7">
         <v>6</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="7">
         <f t="shared" si="18"/>
         <v>24128.472805023193</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="7">
         <v>50</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="7">
         <v>18</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="7">
         <f t="shared" si="19"/>
         <v>21715625.524520874</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="7">
         <f t="shared" si="20"/>
         <v>21206.665551289916</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="7">
         <f t="shared" si="21"/>
         <v>15455.961227416992</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="7">
         <f t="shared" si="22"/>
         <v>15.093712136149406</v>
       </c>
@@ -1722,56 +1753,56 @@
       <c r="A13">
         <v>150</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="7">
         <f t="shared" si="12"/>
         <v>3.771856427192688</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="7">
         <f t="shared" si="13"/>
         <v>15.087425708770752</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="7">
         <f t="shared" si="14"/>
         <v>91770.172119140625</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="7">
         <f t="shared" si="15"/>
         <v>1529.5028686523438</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="7">
         <f t="shared" si="16"/>
         <v>6372.9286193847656</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="7">
         <f t="shared" si="17"/>
         <v>2125</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="7">
         <v>6</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="7">
         <f t="shared" si="18"/>
         <v>48091.169446706772</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="7">
         <v>50</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="7">
         <v>18</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="7">
         <f t="shared" si="19"/>
         <v>43282052.502036095</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="7">
         <f t="shared" si="20"/>
         <v>42267.629396519624</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="7">
         <f t="shared" si="21"/>
         <v>20368.024706840515</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="7">
         <f t="shared" si="22"/>
         <v>19.890649127773941</v>
       </c>
@@ -1784,56 +1815,56 @@
       <c r="A14">
         <v>76</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="7">
         <f t="shared" si="12"/>
         <v>0.24856758117675781</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="7">
         <f t="shared" si="13"/>
         <v>0.99427032470703125</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="7">
         <f t="shared" si="14"/>
         <v>1552.5140729999996</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="7">
         <f t="shared" si="15"/>
         <v>25.875234549999995</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="7">
         <f t="shared" si="16"/>
         <v>107.81347729166664</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="7">
         <f t="shared" si="17"/>
         <v>36</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="7">
         <v>6</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="7">
         <f t="shared" si="18"/>
         <v>53.690597534179688</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="7">
         <v>50</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="7">
         <v>18</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="7">
         <f t="shared" si="19"/>
         <v>48321.537780761719</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="7">
         <f t="shared" si="20"/>
         <v>47.189001739025116</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="7">
         <f t="shared" si="21"/>
         <v>1342.2649383544922</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="7">
         <f t="shared" si="22"/>
         <v>1.3108056038618088</v>
       </c>
@@ -1846,56 +1877,56 @@
       <c r="A15" s="2">
         <v>60</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="7">
         <f t="shared" si="12"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="7">
         <f t="shared" si="13"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="7">
         <f t="shared" si="14"/>
         <v>375.890625</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="7">
         <f t="shared" si="15"/>
         <v>6.2648437499999998</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="7">
         <f t="shared" si="16"/>
         <v>26.103515625</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="7">
         <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="7">
         <v>6</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="7">
         <f t="shared" si="18"/>
         <v>5.2142143249511719</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="7">
         <v>50</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="7">
         <v>18</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="7">
         <f t="shared" si="19"/>
         <v>4692.7928924560547</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="7">
         <f t="shared" si="20"/>
         <v>4.5828055590391159</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="7">
         <f t="shared" si="21"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="7">
         <f t="shared" si="22"/>
         <v>0.50920061767101288</v>
       </c>
@@ -1919,7 +1950,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1">
@@ -1936,7 +1967,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1960,16 +1991,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -2201,7 +2232,7 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -2212,7 +2243,7 @@
     </row>
     <row r="2" ht="14.25">
       <c r="D2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2223,7 +2254,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="G3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -2234,7 +2265,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="G4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -2245,7 +2276,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="G6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2256,7 +2287,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="G7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -2267,7 +2298,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="G8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -2278,7 +2309,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="D10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -2289,7 +2320,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="G11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -2300,7 +2331,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="G12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -2311,7 +2342,7 @@
     </row>
     <row r="14" ht="14.25">
       <c r="G14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2">
         <v>1</v>
@@ -2322,7 +2353,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="G15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H15" s="2">
         <v>1</v>
@@ -2333,7 +2364,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="G16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>
@@ -2347,25 +2378,25 @@
     <row r="19" ht="14.25"/>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" ht="14.25">

</xml_diff>

<commit_message>
Added support for using different datatypes while averaging.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>L</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">For 28 L^2 Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float 28L^2 Size</t>
   </si>
   <si>
     <t xml:space="preserve">Real Size L^2xL^2 (in GB)</t>
@@ -169,19 +172,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -924,32 +921,54 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2">
         <f>(28/4)*B7</f>
         <v>20.861625671386719</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <f>(28/4)*C7</f>
         <v>0.5340576171875</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="2">
         <f>(28/4)*D7</f>
         <v>13.687312602996826</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <f>(28/4)*E7</f>
         <v>8.544921875</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <f>(28/4)*F7</f>
         <v>2.7036666870117188</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="F13" s="2"/>
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f>B12/2</f>
+        <v>10.430812835693359</v>
+      </c>
+      <c r="C13">
+        <f>C12/2</f>
+        <v>0.26702880859375</v>
+      </c>
+      <c r="D13">
+        <f>D12/2</f>
+        <v>6.8436563014984131</v>
+      </c>
+      <c r="E13">
+        <f>E12/2</f>
+        <v>4.2724609375</v>
+      </c>
+      <c r="F13">
+        <f>F12/2</f>
+        <v>1.3518333435058594</v>
+      </c>
     </row>
     <row r="14" ht="14.25">
       <c r="B14">
@@ -1018,109 +1037,109 @@
     <col bestFit="1" min="13" max="14" width="9.4609375"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="85.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="4" customFormat="1" ht="85.5">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
         <v>40</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <f t="shared" ref="B2:B9" si="0">A2^4*8/2^30</f>
         <v>0.019073486328125</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <f t="shared" ref="C2:C9" si="1">4*B2</f>
         <v>0.0762939453125</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <v>33</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <f t="shared" ref="E2:E9" si="2">D2/60</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <f t="shared" ref="F2:F9" si="3">D2*100/(60*24)</f>
         <v>2.2916666666666665</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <f t="shared" ref="G2:G9" si="4">CEILING(MAX(F2/3,1),1)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="5">
         <v>6</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5">
         <f t="shared" ref="I2:I9" si="5">H2*G2*B2</f>
         <v>0.11444091796875</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="5">
         <v>50</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="5">
         <v>18</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="5">
         <f t="shared" ref="L2:L9" si="6">I2*J2*K2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="5">
         <f t="shared" ref="M2:M9" si="7">L2/1024</f>
         <v>0.10058283805847168</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="5">
         <f t="shared" ref="N2:N9" si="8">L2/G2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="5">
         <f t="shared" ref="O2:O9" si="9">N2/1024</f>
         <v>0.10058283805847168</v>
       </c>
@@ -1133,56 +1152,56 @@
       <c r="A3">
         <v>50</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <f t="shared" si="0"/>
         <v>0.046566128730773926</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <f t="shared" si="1"/>
         <v>0.1862645149230957</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <f t="shared" ref="D3:D9" si="11">$D$2*(A3/$A$2)^6</f>
         <v>125.885009765625</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <f t="shared" si="2"/>
         <v>2.09808349609375</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <f t="shared" si="3"/>
         <v>8.7420145670572911</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>6</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <f t="shared" si="5"/>
         <v>0.83819031715393066</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="5">
         <v>50</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="5">
         <v>18</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="5">
         <f t="shared" si="6"/>
         <v>754.3712854385376</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="5">
         <f t="shared" si="7"/>
         <v>0.73669070843607187</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="5">
         <f t="shared" si="8"/>
         <v>251.4570951461792</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="5">
         <f t="shared" si="9"/>
         <v>0.24556356947869062</v>
       </c>
@@ -1195,56 +1214,56 @@
       <c r="A4">
         <v>60</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <f t="shared" si="0"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <f t="shared" si="1"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <f t="shared" si="11"/>
         <v>375.890625</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <f t="shared" si="2"/>
         <v>6.2648437499999998</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <f t="shared" si="3"/>
         <v>26.103515625</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>6</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <f t="shared" si="5"/>
         <v>5.2142143249511719</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <v>50</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="5">
         <v>18</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="5">
         <f t="shared" si="6"/>
         <v>4692.7928924560547</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="5">
         <f t="shared" si="7"/>
         <v>4.5828055590391159</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="5">
         <f t="shared" si="8"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="5">
         <f t="shared" si="9"/>
         <v>0.50920061767101288</v>
       </c>
@@ -1257,56 +1276,56 @@
       <c r="A5">
         <v>70</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <f t="shared" si="0"/>
         <v>0.17888844013214111</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <f t="shared" si="1"/>
         <v>0.71555376052856445</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <f t="shared" si="11"/>
         <v>947.855712890625</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <f t="shared" si="2"/>
         <v>15.797595214843749</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <f t="shared" si="3"/>
         <v>65.823313395182296</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>6</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <f t="shared" si="5"/>
         <v>23.613274097442627</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <v>50</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="5">
         <v>18</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="5">
         <f t="shared" si="6"/>
         <v>21251.946687698364</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="5">
         <f t="shared" si="7"/>
         <v>20.753854187205434</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="5">
         <f t="shared" si="8"/>
         <v>965.99757671356201</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="5">
         <f t="shared" si="9"/>
         <v>0.9433570085093379</v>
       </c>
@@ -1319,56 +1338,56 @@
       <c r="A6">
         <v>80</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <f t="shared" si="0"/>
         <v>0.30517578125</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <f t="shared" si="1"/>
         <v>1.220703125</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <f t="shared" si="11"/>
         <v>2112</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <f t="shared" si="2"/>
         <v>35.200000000000003</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <f t="shared" si="3"/>
         <v>146.66666666666666</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>6</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <f t="shared" si="5"/>
         <v>89.7216796875</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <v>50</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="5">
         <v>18</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="5">
         <f t="shared" si="6"/>
         <v>80749.51171875</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="5">
         <f t="shared" si="7"/>
         <v>78.856945037841797</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="5">
         <f t="shared" si="8"/>
         <v>1647.94921875</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="5">
         <f t="shared" si="9"/>
         <v>1.6093254089355469</v>
       </c>
@@ -1381,56 +1400,56 @@
       <c r="A7">
         <v>90</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <f t="shared" si="0"/>
         <v>0.48883259296417236</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <f t="shared" si="1"/>
         <v>1.9553303718566895</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <f t="shared" si="11"/>
         <v>4281.629150390625</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <f t="shared" si="2"/>
         <v>71.360485839843747</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <f t="shared" si="3"/>
         <v>297.33535766601562</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>6</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5">
         <f t="shared" si="5"/>
         <v>293.29955577850342</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="5">
         <v>50</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="5">
         <v>18</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="5">
         <f t="shared" si="6"/>
         <v>263969.60020065308</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="5">
         <f t="shared" si="7"/>
         <v>257.78281269595027</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="5">
         <f t="shared" si="8"/>
         <v>2639.6960020065308</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="5">
         <f t="shared" si="9"/>
         <v>2.5778281269595027</v>
       </c>
@@ -1443,56 +1462,56 @@
       <c r="A8">
         <v>100</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <f t="shared" si="0"/>
         <v>0.74505805969238281</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <f t="shared" si="1"/>
         <v>2.9802322387695312</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <f t="shared" si="11"/>
         <v>8056.640625</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <f t="shared" si="2"/>
         <v>134.27734375</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <f t="shared" si="3"/>
         <v>559.48893229166663</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <f t="shared" si="4"/>
         <v>187</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <v>6</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <f t="shared" si="5"/>
         <v>835.95514297485352</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <v>1</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="5">
         <v>231</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="5">
         <f t="shared" si="6"/>
         <v>193105.63802719116</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="5">
         <f t="shared" si="7"/>
         <v>188.57972463592887</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="5">
         <f t="shared" si="8"/>
         <v>1032.6504707336426</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="5">
         <f t="shared" si="9"/>
         <v>1.0084477253258228</v>
       </c>
@@ -1505,56 +1524,56 @@
       <c r="A9">
         <v>110</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <f t="shared" si="0"/>
         <v>1.0908395051956177</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <f t="shared" si="1"/>
         <v>4.3633580207824707</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <f t="shared" si="11"/>
         <v>14272.830322265625</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <f t="shared" si="2"/>
         <v>237.88050537109376</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <f t="shared" si="3"/>
         <v>991.16877237955725</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <f t="shared" si="4"/>
         <v>331</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>6</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <f t="shared" si="5"/>
         <v>2166.4072573184967</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <v>50</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="5">
         <v>18</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="5">
         <f t="shared" si="6"/>
         <v>1949766.531586647</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="5">
         <f t="shared" si="7"/>
         <v>1904.068878502585</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="5">
         <f t="shared" si="8"/>
         <v>5890.5333280563354</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="5">
         <f t="shared" si="9"/>
         <v>5.7524739531800151</v>
       </c>
@@ -1567,56 +1586,56 @@
       <c r="A10">
         <v>120</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <f t="shared" ref="B10:B15" si="12">A10^4*8/2^30</f>
         <v>1.544952392578125</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <f t="shared" ref="C10:C15" si="13">4*B10</f>
         <v>6.1798095703125</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <f t="shared" ref="D10:D15" si="14">$D$2*(A10/$A$2)^6</f>
         <v>24057</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <f t="shared" ref="E10:E15" si="15">D10/60</f>
         <v>400.94999999999999</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <f t="shared" ref="F10:F15" si="16">D10*100/(60*24)</f>
         <v>1670.625</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <f t="shared" ref="G10:G15" si="17">CEILING(MAX(F10/3,1),1)</f>
         <v>557</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>6</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="5">
         <f t="shared" ref="I10:I15" si="18">H10*G10*B10</f>
         <v>5163.2308959960938</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <v>50</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="5">
         <v>18</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="5">
         <f t="shared" ref="L10:L15" si="19">I10*J10*K10</f>
         <v>4646907.8063964844</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="5">
         <f t="shared" ref="M10:M15" si="20">L10/1024</f>
         <v>4537.9959046840668</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="5">
         <f t="shared" ref="N10:N15" si="21">L10/G10</f>
         <v>8342.742919921875</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="5">
         <f t="shared" ref="O10:O15" si="22">N10/1024</f>
         <v>8.1472098827362061</v>
       </c>
@@ -1629,56 +1648,56 @@
       <c r="A11">
         <v>130</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <f t="shared" si="12"/>
         <v>2.1279603242874146</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <f t="shared" si="13"/>
         <v>8.5118412971496582</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <f t="shared" si="14"/>
         <v>38887.865478515625</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <f t="shared" si="15"/>
         <v>648.1310913085938</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <f t="shared" si="16"/>
         <v>2700.5462137858071</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <f t="shared" si="17"/>
         <v>901</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>6</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="5">
         <f t="shared" si="18"/>
         <v>11503.753513097763</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="5">
         <v>50</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="5">
         <v>18</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="5">
         <f t="shared" si="19"/>
         <v>10353378.161787987</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="5">
         <f t="shared" si="20"/>
         <v>10110.720861121081</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="5">
         <f t="shared" si="21"/>
         <v>11490.985751152039</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="5">
         <f t="shared" si="22"/>
         <v>11.221665772609413</v>
       </c>
@@ -1691,56 +1710,56 @@
       <c r="A12">
         <v>140</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <f t="shared" si="12"/>
         <v>2.8622150421142578</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <f t="shared" si="13"/>
         <v>11.448860168457031</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <f t="shared" si="14"/>
         <v>60662.765625</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <f t="shared" si="15"/>
         <v>1011.04609375</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <f t="shared" si="16"/>
         <v>4212.692057291667</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <f t="shared" si="17"/>
         <v>1405</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>6</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="5">
         <f t="shared" si="18"/>
         <v>24128.472805023193</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <v>50</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="5">
         <v>18</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="5">
         <f t="shared" si="19"/>
         <v>21715625.524520874</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="5">
         <f t="shared" si="20"/>
         <v>21206.665551289916</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="5">
         <f t="shared" si="21"/>
         <v>15455.961227416992</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="5">
         <f t="shared" si="22"/>
         <v>15.093712136149406</v>
       </c>
@@ -1753,56 +1772,56 @@
       <c r="A13">
         <v>150</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <f t="shared" si="12"/>
         <v>3.771856427192688</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <f t="shared" si="13"/>
         <v>15.087425708770752</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <f t="shared" si="14"/>
         <v>91770.172119140625</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <f t="shared" si="15"/>
         <v>1529.5028686523438</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <f t="shared" si="16"/>
         <v>6372.9286193847656</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="5">
         <f t="shared" si="17"/>
         <v>2125</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <v>6</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="5">
         <f t="shared" si="18"/>
         <v>48091.169446706772</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <v>50</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="5">
         <v>18</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="5">
         <f t="shared" si="19"/>
         <v>43282052.502036095</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="5">
         <f t="shared" si="20"/>
         <v>42267.629396519624</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="5">
         <f t="shared" si="21"/>
         <v>20368.024706840515</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="5">
         <f t="shared" si="22"/>
         <v>19.890649127773941</v>
       </c>
@@ -1815,56 +1834,56 @@
       <c r="A14">
         <v>76</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <f t="shared" si="12"/>
         <v>0.24856758117675781</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <f t="shared" si="13"/>
         <v>0.99427032470703125</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <f t="shared" si="14"/>
         <v>1552.5140729999996</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <f t="shared" si="15"/>
         <v>25.875234549999995</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <f t="shared" si="16"/>
         <v>107.81347729166664</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="5">
         <f t="shared" si="17"/>
         <v>36</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>6</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="5">
         <f t="shared" si="18"/>
         <v>53.690597534179688</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <v>50</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="5">
         <v>18</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="5">
         <f t="shared" si="19"/>
         <v>48321.537780761719</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="5">
         <f t="shared" si="20"/>
         <v>47.189001739025116</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="5">
         <f t="shared" si="21"/>
         <v>1342.2649383544922</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="5">
         <f t="shared" si="22"/>
         <v>1.3108056038618088</v>
       </c>
@@ -1877,56 +1896,56 @@
       <c r="A15" s="2">
         <v>60</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <f t="shared" si="12"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <f t="shared" si="13"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <f t="shared" si="14"/>
         <v>375.890625</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <f t="shared" si="15"/>
         <v>6.2648437499999998</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <f t="shared" si="16"/>
         <v>26.103515625</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="5">
         <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="5">
         <v>6</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="5">
         <f t="shared" si="18"/>
         <v>5.2142143249511719</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="5">
         <v>50</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="5">
         <v>18</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="5">
         <f t="shared" si="19"/>
         <v>4692.7928924560547</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="5">
         <f t="shared" si="20"/>
         <v>4.5828055590391159</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="5">
         <f t="shared" si="21"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="5">
         <f t="shared" si="22"/>
         <v>0.50920061767101288</v>
       </c>
@@ -1991,16 +2010,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -2232,7 +2251,7 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -2243,7 +2262,7 @@
     </row>
     <row r="2" ht="14.25">
       <c r="D2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2254,7 +2273,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="G3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -2265,7 +2284,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="G4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -2276,7 +2295,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="G6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2287,7 +2306,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="G7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -2298,7 +2317,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="G8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -2309,7 +2328,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="D10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -2320,7 +2339,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="G11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -2331,7 +2350,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="G12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -2342,7 +2361,7 @@
     </row>
     <row r="14" ht="14.25">
       <c r="G14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H14" s="2">
         <v>1</v>
@@ -2353,7 +2372,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="G15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H15" s="2">
         <v>1</v>
@@ -2364,7 +2383,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="G16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>
@@ -2378,25 +2397,25 @@
     <row r="19" ht="14.25"/>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" ht="14.25">

</xml_diff>

<commit_message>
Keldysh statistics implemented correctly.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -11,14 +11,15 @@
     <sheet name="Sheet6" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>L</t>
   </si>
@@ -53,6 +54,9 @@
     <t xml:space="preserve">Float 28L^2 Size</t>
   </si>
   <si>
+    <t xml:space="preserve">Float 36L^2 Size</t>
+  </si>
+  <si>
     <t xml:space="preserve">Real Size L^2xL^2 (in GB)</t>
   </si>
   <si>
@@ -135,6 +139,24 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>G00</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G01</t>
+  </si>
+  <si>
+    <t>Var00</t>
+  </si>
+  <si>
+    <t>Var11</t>
+  </si>
+  <si>
+    <t>Var01</t>
   </si>
 </sst>
 </file>
@@ -146,9 +168,9 @@
   </numFmts>
   <fonts count="1">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -172,17 +194,26 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,23 +930,23 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <f>6*B7</f>
         <v>17.881393432617188</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <f>6*C7</f>
         <v>0.457763671875</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <f>6*D7</f>
         <v>11.731982231140137</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <f>6*E7</f>
         <v>7.32421875</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="5">
         <f>6*F7</f>
         <v>2.3174285888671875</v>
       </c>
@@ -924,23 +955,23 @@
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <f>(28/4)*B7</f>
         <v>20.861625671386719</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="5">
         <f>(28/4)*C7</f>
         <v>0.5340576171875</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="5">
         <f>(28/4)*D7</f>
         <v>13.687312602996826</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <f>(28/4)*E7</f>
         <v>8.544921875</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="5">
         <f>(28/4)*F7</f>
         <v>2.7036666870117188</v>
       </c>
@@ -949,75 +980,106 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <f>B12/2</f>
         <v>10.430812835693359</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <f>C12/2</f>
         <v>0.26702880859375</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <f>D12/2</f>
         <v>6.8436563014984131</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <f>E12/2</f>
         <v>4.2724609375</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="4">
         <f>F12/2</f>
         <v>1.3518333435058594</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="B14">
+      <c r="B14" s="4">
         <f>50*(4+2)*B7*2</f>
         <v>1788.1393432617188</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <f>50*(4+2)*C7*2</f>
         <v>45.7763671875</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <f>50*(4+2)*D7*2</f>
         <v>1173.1982231140137</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <f>50*(4+2)*E7*2</f>
         <v>732.421875</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="5">
         <f>50*(4+2)*F7*2</f>
         <v>231.74285888671875</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="B15">
+      <c r="B15" s="4">
         <f>B14*18/1024</f>
         <v>31.4321368932724</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <f>C14*18/1024</f>
         <v>0.80466270446777344</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <f>D14*18/1024</f>
         <v>20.622625015676022</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <f>E14*18/1024</f>
         <v>12.874603271484375</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="5">
         <f>F14*18/1024</f>
         <v>4.073604941368103</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4">
+        <f>36*B7/(2*4)</f>
+        <v>13.411045074462891</v>
+      </c>
+      <c r="C16" s="4">
+        <f>36*C7/(2*4)</f>
+        <v>0.34332275390625</v>
+      </c>
+      <c r="D16" s="4">
+        <f>36*D7/(2*4)</f>
+        <v>8.7989866733551025</v>
+      </c>
+      <c r="E16" s="4">
+        <f>36*E7/(2*4)</f>
+        <v>5.4931640625</v>
+      </c>
+      <c r="F16" s="4">
+        <f>36*F7/(2*4)</f>
+        <v>1.7380714416503906</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="3">
+        <f>12+(B8+B7+B7)/4</f>
+        <v>14.980232238769531</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1037,109 +1099,109 @@
     <col bestFit="1" min="13" max="14" width="9.4609375"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="85.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="6" customFormat="1" ht="85.5">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
         <v>40</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <f t="shared" ref="B2:B9" si="0">A2^4*8/2^30</f>
         <v>0.019073486328125</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <f t="shared" ref="C2:C9" si="1">4*B2</f>
         <v>0.0762939453125</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>33</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f t="shared" ref="E2:E9" si="2">D2/60</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <f t="shared" ref="F2:F9" si="3">D2*100/(60*24)</f>
         <v>2.2916666666666665</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <f t="shared" ref="G2:G9" si="4">CEILING(MAX(F2/3,1),1)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>6</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <f t="shared" ref="I2:I9" si="5">H2*G2*B2</f>
         <v>0.11444091796875</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>50</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>18</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <f t="shared" ref="L2:L9" si="6">I2*J2*K2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <f t="shared" ref="M2:M9" si="7">L2/1024</f>
         <v>0.10058283805847168</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="4">
         <f t="shared" ref="N2:N9" si="8">L2/G2</f>
         <v>102.996826171875</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <f t="shared" ref="O2:O9" si="9">N2/1024</f>
         <v>0.10058283805847168</v>
       </c>
@@ -1152,56 +1214,56 @@
       <c r="A3">
         <v>50</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <f t="shared" si="0"/>
         <v>0.046566128730773926</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <f t="shared" si="1"/>
         <v>0.1862645149230957</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <f t="shared" ref="D3:D9" si="11">$D$2*(A3/$A$2)^6</f>
         <v>125.885009765625</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <f t="shared" si="2"/>
         <v>2.09808349609375</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f t="shared" si="3"/>
         <v>8.7420145670572911</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>6</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <f t="shared" si="5"/>
         <v>0.83819031715393066</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>50</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>18</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <f t="shared" si="6"/>
         <v>754.3712854385376</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <f t="shared" si="7"/>
         <v>0.73669070843607187</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <f t="shared" si="8"/>
         <v>251.4570951461792</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="4">
         <f t="shared" si="9"/>
         <v>0.24556356947869062</v>
       </c>
@@ -1214,56 +1276,56 @@
       <c r="A4">
         <v>60</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <f t="shared" si="0"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <f t="shared" si="1"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <f t="shared" si="11"/>
         <v>375.890625</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f t="shared" si="2"/>
         <v>6.2648437499999998</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f t="shared" si="3"/>
         <v>26.103515625</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>6</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <f t="shared" si="5"/>
         <v>5.2142143249511719</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>50</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>18</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <f t="shared" si="6"/>
         <v>4692.7928924560547</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <f t="shared" si="7"/>
         <v>4.5828055590391159</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <f t="shared" si="8"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <f t="shared" si="9"/>
         <v>0.50920061767101288</v>
       </c>
@@ -1276,56 +1338,56 @@
       <c r="A5">
         <v>70</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <f t="shared" si="0"/>
         <v>0.17888844013214111</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <f t="shared" si="1"/>
         <v>0.71555376052856445</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <f t="shared" si="11"/>
         <v>947.855712890625</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <f t="shared" si="2"/>
         <v>15.797595214843749</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f t="shared" si="3"/>
         <v>65.823313395182296</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>6</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <f t="shared" si="5"/>
         <v>23.613274097442627</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>50</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>18</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <f t="shared" si="6"/>
         <v>21251.946687698364</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <f t="shared" si="7"/>
         <v>20.753854187205434</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <f t="shared" si="8"/>
         <v>965.99757671356201</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="4">
         <f t="shared" si="9"/>
         <v>0.9433570085093379</v>
       </c>
@@ -1338,56 +1400,56 @@
       <c r="A6">
         <v>80</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <f t="shared" si="0"/>
         <v>0.30517578125</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <f t="shared" si="1"/>
         <v>1.220703125</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f t="shared" si="11"/>
         <v>2112</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <f t="shared" si="2"/>
         <v>35.200000000000003</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f t="shared" si="3"/>
         <v>146.66666666666666</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>6</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <f t="shared" si="5"/>
         <v>89.7216796875</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>50</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>18</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <f t="shared" si="6"/>
         <v>80749.51171875</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <f t="shared" si="7"/>
         <v>78.856945037841797</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <f t="shared" si="8"/>
         <v>1647.94921875</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="4">
         <f t="shared" si="9"/>
         <v>1.6093254089355469</v>
       </c>
@@ -1400,56 +1462,56 @@
       <c r="A7">
         <v>90</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f t="shared" si="0"/>
         <v>0.48883259296417236</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <f t="shared" si="1"/>
         <v>1.9553303718566895</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <f t="shared" si="11"/>
         <v>4281.629150390625</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f t="shared" si="2"/>
         <v>71.360485839843747</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f t="shared" si="3"/>
         <v>297.33535766601562</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>6</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <f t="shared" si="5"/>
         <v>293.29955577850342</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>50</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>18</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <f t="shared" si="6"/>
         <v>263969.60020065308</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <f t="shared" si="7"/>
         <v>257.78281269595027</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <f t="shared" si="8"/>
         <v>2639.6960020065308</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="4">
         <f t="shared" si="9"/>
         <v>2.5778281269595027</v>
       </c>
@@ -1462,56 +1524,56 @@
       <c r="A8">
         <v>100</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <f t="shared" si="0"/>
         <v>0.74505805969238281</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <f t="shared" si="1"/>
         <v>2.9802322387695312</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <f t="shared" si="11"/>
         <v>8056.640625</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" si="2"/>
         <v>134.27734375</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" si="3"/>
         <v>559.48893229166663</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f t="shared" si="4"/>
         <v>187</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>6</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <f t="shared" si="5"/>
         <v>835.95514297485352</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>1</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>231</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <f t="shared" si="6"/>
         <v>193105.63802719116</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <f t="shared" si="7"/>
         <v>188.57972463592887</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <f t="shared" si="8"/>
         <v>1032.6504707336426</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="4">
         <f t="shared" si="9"/>
         <v>1.0084477253258228</v>
       </c>
@@ -1524,56 +1586,56 @@
       <c r="A9">
         <v>110</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <f t="shared" si="0"/>
         <v>1.0908395051956177</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <f t="shared" si="1"/>
         <v>4.3633580207824707</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <f t="shared" si="11"/>
         <v>14272.830322265625</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <f t="shared" si="2"/>
         <v>237.88050537109376</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f t="shared" si="3"/>
         <v>991.16877237955725</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f t="shared" si="4"/>
         <v>331</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>6</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <f t="shared" si="5"/>
         <v>2166.4072573184967</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>50</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="4">
         <v>18</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="4">
         <f t="shared" si="6"/>
         <v>1949766.531586647</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <f t="shared" si="7"/>
         <v>1904.068878502585</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="4">
         <f t="shared" si="8"/>
         <v>5890.5333280563354</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="4">
         <f t="shared" si="9"/>
         <v>5.7524739531800151</v>
       </c>
@@ -1586,56 +1648,56 @@
       <c r="A10">
         <v>120</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <f t="shared" ref="B10:B15" si="12">A10^4*8/2^30</f>
         <v>1.544952392578125</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <f t="shared" ref="C10:C15" si="13">4*B10</f>
         <v>6.1798095703125</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <f t="shared" ref="D10:D15" si="14">$D$2*(A10/$A$2)^6</f>
         <v>24057</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" ref="E10:E15" si="15">D10/60</f>
         <v>400.94999999999999</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f t="shared" ref="F10:F15" si="16">D10*100/(60*24)</f>
         <v>1670.625</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f t="shared" ref="G10:G15" si="17">CEILING(MAX(F10/3,1),1)</f>
         <v>557</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>6</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <f t="shared" ref="I10:I15" si="18">H10*G10*B10</f>
         <v>5163.2308959960938</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>50</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="4">
         <v>18</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <f t="shared" ref="L10:L15" si="19">I10*J10*K10</f>
         <v>4646907.8063964844</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <f t="shared" ref="M10:M15" si="20">L10/1024</f>
         <v>4537.9959046840668</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="4">
         <f t="shared" ref="N10:N15" si="21">L10/G10</f>
         <v>8342.742919921875</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="4">
         <f t="shared" ref="O10:O15" si="22">N10/1024</f>
         <v>8.1472098827362061</v>
       </c>
@@ -1648,56 +1710,56 @@
       <c r="A11">
         <v>130</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <f t="shared" si="12"/>
         <v>2.1279603242874146</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <f t="shared" si="13"/>
         <v>8.5118412971496582</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f t="shared" si="14"/>
         <v>38887.865478515625</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="15"/>
         <v>648.1310913085938</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f t="shared" si="16"/>
         <v>2700.5462137858071</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f t="shared" si="17"/>
         <v>901</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>6</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <f t="shared" si="18"/>
         <v>11503.753513097763</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <v>50</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <v>18</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <f t="shared" si="19"/>
         <v>10353378.161787987</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <f t="shared" si="20"/>
         <v>10110.720861121081</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="4">
         <f t="shared" si="21"/>
         <v>11490.985751152039</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="4">
         <f t="shared" si="22"/>
         <v>11.221665772609413</v>
       </c>
@@ -1710,56 +1772,56 @@
       <c r="A12">
         <v>140</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <f t="shared" si="12"/>
         <v>2.8622150421142578</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <f t="shared" si="13"/>
         <v>11.448860168457031</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <f t="shared" si="14"/>
         <v>60662.765625</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f t="shared" si="15"/>
         <v>1011.04609375</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f t="shared" si="16"/>
         <v>4212.692057291667</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f t="shared" si="17"/>
         <v>1405</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>6</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <f t="shared" si="18"/>
         <v>24128.472805023193</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <v>50</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="4">
         <v>18</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <f t="shared" si="19"/>
         <v>21715625.524520874</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="4">
         <f t="shared" si="20"/>
         <v>21206.665551289916</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="4">
         <f t="shared" si="21"/>
         <v>15455.961227416992</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="4">
         <f t="shared" si="22"/>
         <v>15.093712136149406</v>
       </c>
@@ -1772,56 +1834,56 @@
       <c r="A13">
         <v>150</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <f t="shared" si="12"/>
         <v>3.771856427192688</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <f t="shared" si="13"/>
         <v>15.087425708770752</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <f t="shared" si="14"/>
         <v>91770.172119140625</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="15"/>
         <v>1529.5028686523438</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" si="16"/>
         <v>6372.9286193847656</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f t="shared" si="17"/>
         <v>2125</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>6</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <f t="shared" si="18"/>
         <v>48091.169446706772</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>50</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <v>18</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <f t="shared" si="19"/>
         <v>43282052.502036095</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="4">
         <f t="shared" si="20"/>
         <v>42267.629396519624</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="4">
         <f t="shared" si="21"/>
         <v>20368.024706840515</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="4">
         <f t="shared" si="22"/>
         <v>19.890649127773941</v>
       </c>
@@ -1834,56 +1896,56 @@
       <c r="A14">
         <v>76</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <f t="shared" si="12"/>
         <v>0.24856758117675781</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <f t="shared" si="13"/>
         <v>0.99427032470703125</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <f t="shared" si="14"/>
         <v>1552.5140729999996</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <f t="shared" si="15"/>
         <v>25.875234549999995</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f t="shared" si="16"/>
         <v>107.81347729166664</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f t="shared" si="17"/>
         <v>36</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>6</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="4">
         <f t="shared" si="18"/>
         <v>53.690597534179688</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="4">
         <v>50</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="4">
         <v>18</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="4">
         <f t="shared" si="19"/>
         <v>48321.537780761719</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="4">
         <f t="shared" si="20"/>
         <v>47.189001739025116</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="4">
         <f t="shared" si="21"/>
         <v>1342.2649383544922</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="4">
         <f t="shared" si="22"/>
         <v>1.3108056038618088</v>
       </c>
@@ -1896,56 +1958,56 @@
       <c r="A15" s="2">
         <v>60</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <f t="shared" si="12"/>
         <v>0.096559524536132812</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <f t="shared" si="13"/>
         <v>0.38623809814453125</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f t="shared" si="14"/>
         <v>375.890625</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f t="shared" si="15"/>
         <v>6.2648437499999998</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f t="shared" si="16"/>
         <v>26.103515625</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>6</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <f t="shared" si="18"/>
         <v>5.2142143249511719</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="4">
         <v>50</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="4">
         <v>18</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="4">
         <f t="shared" si="19"/>
         <v>4692.7928924560547</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="4">
         <f t="shared" si="20"/>
         <v>4.5828055590391159</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="4">
         <f t="shared" si="21"/>
         <v>521.42143249511719</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="4">
         <f t="shared" si="22"/>
         <v>0.50920061767101288</v>
       </c>
@@ -1957,7 +2019,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1986,7 +2048,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2010,16 +2072,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
@@ -2235,7 +2297,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2251,7 +2313,7 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -2262,7 +2324,7 @@
     </row>
     <row r="2" ht="14.25">
       <c r="D2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2273,7 +2335,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="G3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -2284,7 +2346,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="G4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -2295,7 +2357,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="G6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2306,7 +2368,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="G7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -2317,7 +2379,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="G8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -2328,7 +2390,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="D10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -2339,7 +2401,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="G11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -2350,7 +2412,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="G12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -2361,7 +2423,7 @@
     </row>
     <row r="14" ht="14.25">
       <c r="G14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2">
         <v>1</v>
@@ -2372,7 +2434,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="G15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H15" s="2">
         <v>1</v>
@@ -2383,7 +2445,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="G16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>
@@ -2397,25 +2459,25 @@
     <row r="19" ht="14.25"/>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" ht="14.25">
@@ -2503,12 +2565,216 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="2">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2">
+        <f>SUM(A2:L2)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="2">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="8">
+        <f>SUM(A3:L3)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="2">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="8">
+        <f>SUM(A4:L4)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="2">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2</v>
+      </c>
+      <c r="M5" s="8">
+        <f>SUM(A5:L5)</f>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
@@ -2523,7 +2789,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added support for initial conds to be directly written as binary.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>L</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t xml:space="preserve">Size Complex (in GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For 4L^2</t>
   </si>
   <si>
     <t xml:space="preserve">For 24 L^2 Size</t>
@@ -163,8 +166,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="160" formatCode="0.0"/>
+    <numFmt numFmtId="161" formatCode="0.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -194,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -202,17 +206,12 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,11 +923,33 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="F10" s="2"/>
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <f>2*B8</f>
+        <v>11.920928955078125</v>
+      </c>
+      <c r="C10" s="5">
+        <f>2*C8</f>
+        <v>0.30517578125</v>
+      </c>
+      <c r="D10" s="5">
+        <f>2*D8</f>
+        <v>7.8213214874267578</v>
+      </c>
+      <c r="E10" s="5">
+        <f>2*E8</f>
+        <v>4.8828125</v>
+      </c>
+      <c r="F10" s="5">
+        <f>2*F8</f>
+        <v>1.544952392578125</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4">
         <f>6*B7</f>
@@ -946,39 +967,39 @@
         <f>6*E7</f>
         <v>7.32421875</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <f>6*F7</f>
         <v>2.3174285888671875</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
         <f>(28/4)*B7</f>
         <v>20.861625671386719</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <f>(28/4)*C7</f>
         <v>0.5340576171875</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <f>(28/4)*D7</f>
         <v>13.687312602996826</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <f>(28/4)*E7</f>
         <v>8.544921875</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <f>(28/4)*F7</f>
         <v>2.7036666870117188</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <f>B12/2</f>
@@ -1018,7 +1039,7 @@
         <f>50*(4+2)*E7*2</f>
         <v>732.421875</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <f>50*(4+2)*F7*2</f>
         <v>231.74285888671875</v>
       </c>
@@ -1040,14 +1061,14 @@
         <f>E14*18/1024</f>
         <v>12.874603271484375</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <f>F14*18/1024</f>
         <v>4.073604941368103</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4">
         <f>36*B7/(2*4)</f>
@@ -1099,54 +1120,54 @@
     <col bestFit="1" min="13" max="14" width="9.4609375"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="85.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="7" customFormat="1" ht="85.5">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>26</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -2072,16 +2093,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -2313,7 +2334,7 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -2324,7 +2345,7 @@
     </row>
     <row r="2" ht="14.25">
       <c r="D2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2335,7 +2356,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="G3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -2346,7 +2367,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="G4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -2357,7 +2378,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="G6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2368,7 +2389,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="G7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -2379,7 +2400,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="G8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -2390,7 +2411,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="D10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -2401,7 +2422,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="G11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -2412,7 +2433,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="G12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -2423,7 +2444,7 @@
     </row>
     <row r="14" ht="14.25">
       <c r="G14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H14" s="2">
         <v>1</v>
@@ -2434,7 +2455,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="G15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H15" s="2">
         <v>1</v>
@@ -2445,7 +2466,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="G16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>
@@ -2459,25 +2480,25 @@
     <row r="19" ht="14.25"/>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" ht="14.25">
@@ -2581,40 +2602,40 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M1" s="2"/>
     </row>
@@ -2650,7 +2671,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2">
-        <f>SUM(A2:L2)</f>
+        <f t="shared" ref="M2:M5" si="32">SUM(A2:L2)</f>
         <v>30</v>
       </c>
     </row>
@@ -2658,7 +2679,7 @@
       <c r="A3" s="2">
         <v>8</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3">
@@ -2687,8 +2708,8 @@
       <c r="L3" s="2">
         <v>2</v>
       </c>
-      <c r="M3" s="8">
-        <f>SUM(A3:L3)</f>
+      <c r="M3" s="2">
+        <f t="shared" si="32"/>
         <v>30</v>
       </c>
     </row>
@@ -2696,7 +2717,7 @@
       <c r="A4" s="2">
         <v>8</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4">
@@ -2723,8 +2744,8 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="8">
-        <f>SUM(A4:L4)</f>
+      <c r="M4" s="2">
+        <f t="shared" si="32"/>
         <v>36</v>
       </c>
     </row>
@@ -2732,7 +2753,7 @@
       <c r="A5" s="2">
         <v>8</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5">
@@ -2761,8 +2782,8 @@
       <c r="L5" s="2">
         <v>2</v>
       </c>
-      <c r="M5" s="8">
-        <f>SUM(A5:L5)</f>
+      <c r="M5" s="2">
+        <f t="shared" si="32"/>
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed memory leak bug in random density calculations.
</commit_message>
<xml_diff>
--- a/docs/matrix_size_calcs.xlsx
+++ b/docs/matrix_size_calcs.xlsx
@@ -166,9 +166,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="160" formatCode="0.0"/>
-    <numFmt numFmtId="161" formatCode="0.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -198,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -206,7 +205,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -927,24 +925,24 @@
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <f>2*B8</f>
-        <v>11.920928955078125</v>
-      </c>
-      <c r="C10" s="5">
-        <f>2*C8</f>
-        <v>0.30517578125</v>
-      </c>
-      <c r="D10" s="5">
-        <f>2*D8</f>
-        <v>7.8213214874267578</v>
-      </c>
-      <c r="E10" s="5">
-        <f>2*E8</f>
-        <v>4.8828125</v>
-      </c>
-      <c r="F10" s="5">
-        <f>2*F8</f>
-        <v>1.544952392578125</v>
+        <f>2*B7</f>
+        <v>5.9604644775390625</v>
+      </c>
+      <c r="C10" s="4">
+        <f>2*C7</f>
+        <v>0.152587890625</v>
+      </c>
+      <c r="D10" s="4">
+        <f>2*D7</f>
+        <v>3.9106607437133789</v>
+      </c>
+      <c r="E10" s="4">
+        <f>2*E7</f>
+        <v>2.44140625</v>
+      </c>
+      <c r="F10" s="4">
+        <f>2*F7</f>
+        <v>0.7724761962890625</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -967,7 +965,7 @@
         <f>6*E7</f>
         <v>7.32421875</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f>6*F7</f>
         <v>2.3174285888671875</v>
       </c>
@@ -976,23 +974,23 @@
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f>(28/4)*B7</f>
         <v>20.861625671386719</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <f>(28/4)*C7</f>
         <v>0.5340576171875</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <f>(28/4)*D7</f>
         <v>13.687312602996826</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <f>(28/4)*E7</f>
         <v>8.544921875</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f>(28/4)*F7</f>
         <v>2.7036666870117188</v>
       </c>
@@ -1039,7 +1037,7 @@
         <f>50*(4+2)*E7*2</f>
         <v>732.421875</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <f>50*(4+2)*F7*2</f>
         <v>231.74285888671875</v>
       </c>
@@ -1061,7 +1059,7 @@
         <f>E14*18/1024</f>
         <v>12.874603271484375</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <f>F14*18/1024</f>
         <v>4.073604941368103</v>
       </c>
@@ -1120,53 +1118,53 @@
     <col bestFit="1" min="13" max="14" width="9.4609375"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="1" ht="85.5">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="6" customFormat="1" ht="85.5">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>